<commit_message>
The dataset was updated and util was fixed
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form.xlsx
+++ b/dataset/Extraction_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3000" windowWidth="38400" windowHeight="24000"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="15260"/>
   </bookViews>
   <sheets>
     <sheet name="Folha 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="639">
   <si>
     <t>Citation</t>
   </si>
@@ -40,10 +40,6 @@
   </si>
   <si>
     <t>Perez et al. 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boris Pe ́rez, Dar ́ıo Correal 
-, Herna ́n Astudillo </t>
   </si>
   <si>
     <r>
@@ -2518,9 +2514,6 @@
   <si>
     <t xml:space="preserve">In future work, we plan to study the process of issue removal to determine which issues are the most costly to remove and generally extend this analysis to a wider range of project domains and sizes. 
 </t>
-  </si>
-  <si>
-    <t>Nayebi 2019</t>
   </si>
   <si>
     <t xml:space="preserve">Maleknaz Nayebi, Yuanfang Cai,Rick Kazman, Guenther Ruhe, Qiong Feng, Chris Carlson, Francis Chew </t>
@@ -11468,9 +11461,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Besker, Martini and Bosch </t>
-  </si>
-  <si>
     <r>
       <rPr>
         <u/>
@@ -12760,9 +12750,6 @@
     <t>Requirements volatility is a major issue in software (SW) development, causing problems such as project delays and cost overruns. Even though there is a considerable amount of research related to requirement volatility, the majority of it is inclined toward project management aspects. The relationship between SW architecture design and requirements volatility has not been researched widely, even though changing requirements may for example lead to higher defect density during testing. An exploratory case study was conducted to study how requirements volatility affects SW architecture design. Fifteen semi-structured, thematic interviews were conducted in the case company, which provides the selection of software products for business customers and consumers. The research revealed the factors, such as requirements uncertainty and dynamic business environment, causing requirements volatility in the case company. The study identified the challenges that requirements volatility posed to SW architecture design, including scheduling and architectural technical debt. In addition, this study discusses means of mitigating the factors that cause requirements volatility and addressing the challenges posed by requirements volatility. SW architects are strongly influenced by requirement volatility. Thus understanding the factors causing requirements volatility as well as means to mitigate the challenges has high industrial relevance.</t>
   </si>
   <si>
-    <t>ICSSP 2017</t>
-  </si>
-  <si>
     <t>Software and System Process</t>
   </si>
   <si>
@@ -12798,32 +12785,6 @@
   </si>
   <si>
     <t>Martini et al 2015</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">Antonio Martini </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="22"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>⇑</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>, Jan Bosch, Michel Chaudron</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Investigating Architectural Technical Debt accumulation and refactoring over time: A multiple-case study </t>
@@ -14467,9 +14428,6 @@
     </r>
   </si>
   <si>
-    <t>Curtis et al2012</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bill Curtis, Jay Sappidi, and Alexandra Szynkarski, </t>
   </si>
   <si>
@@ -15978,12 +15936,98 @@
   <si>
     <t>Weak Aspects</t>
   </si>
+  <si>
+    <t>Nayebi et al. 2019</t>
+  </si>
+  <si>
+    <t>Curtis et al 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan MacCormack, Daniel J. Sturtevant </t>
+  </si>
+  <si>
+    <t>MacComark and Sturteant 2016</t>
+  </si>
+  <si>
+    <t>Besker, Martini and Bosch 2017</t>
+  </si>
+  <si>
+    <t>Damian A. Tamburri 2019</t>
+  </si>
+  <si>
+    <t>Boris Perez; Dario Correal; Hernan Astudillo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>Antonio Martini</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>, Jan Bosch, Michel Chaudron</t>
+    </r>
+  </si>
+  <si>
+    <t>Jeremy Ludwig; Steven Xu; Frederick Webber</t>
+  </si>
+  <si>
+    <t>Confernce</t>
+  </si>
+  <si>
+    <t>Conferene</t>
+  </si>
+  <si>
+    <t>Symposium</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>ICSSP 2017 Proceedings of the 2017 International Conference on Software and System Process</t>
+  </si>
+  <si>
+    <t>Book series</t>
+  </si>
+  <si>
+    <t>Measurement,Social networking (online),Computer architecture,Software architecture,Software systems,Software design</t>
+  </si>
+  <si>
+    <t>Identify architectural smells using SNA (Social Network Analysis) via graph based approuch to make predictions about software design dependencies, evolution and properties of the system.</t>
+  </si>
+  <si>
+    <t>Not available</t>
+  </si>
+  <si>
+    <t>The ongoing research has primary focused on the definition of the dependency graph and the evaluation of the depend- ency predictor. The definition of the dependency graph was complemented with a statistical analysis of software versions and the evolution of SNA metrics (tackling RQ1). In this line, it was analysed how past decisions reflected in the software structure affect the future occurrence of dependencies, and smells thereof (tackling RQ3). In addition, it was analysed the descriptive power of both topological and content-based fea- tures for defining the similarity of components (tackling RQ2). The descriptive power of software-related metrics remains to be evaluated. Regarding smell prediction, evaluations focused on defining preliminary filtering strategies for cycles and hubs (tackling RQ4).
+At present, the research is oriented to perform a systematic study with more systems (and versions) to corroborate the initial findings reported in [9, 10]. Moreover, considering the errors in which learned models could incur, additional studies are being performed to introduce mechanisms of reinforcement learning to feed the predictions with new information obtained from the environment (or from the architect), as a means to establish the confidence of predictions and reducing the probability of false positives.
+Once the prediction technique is fully evaluated, it will be incorporated into a tool to evaluate the capabilities of the approach in a study with subjects in the context of real software projects. Finally, it is expected to include other types of architectural smells [15] in the work.</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Software architecture health monitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilateral cloud security architecture Design smells Technical debt Design debt Cloud computing security Design refactoring </t>
+  </si>
+  <si>
+    <t>Computer architecture,Software engineering,Business,History,Sonar detection,Microprocessors</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="56" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -16218,11 +16262,6 @@
       <sz val="24"/>
       <color indexed="14"/>
       <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="22"/>
-      <name val="Times Roman"/>
     </font>
     <font>
       <sz val="9"/>
@@ -16570,10 +16609,7 @@
     <xf numFmtId="49" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -16602,7 +16638,7 @@
     <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="50" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="49" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -16610,6 +16646,9 @@
     </xf>
     <xf numFmtId="49" fontId="42" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17762,9 +17801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -17775,7 +17814,7 @@
     <col min="4" max="4" width="23.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="53" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="72.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="102.83203125" style="1" customWidth="1"/>
     <col min="8" max="9" width="33.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="1" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
@@ -17796,7 +17835,7 @@
   <sheetData>
     <row r="1" spans="1:28" ht="28" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -17805,52 +17844,52 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>4</v>
@@ -17859,28 +17898,28 @@
         <v>5</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="409.5" customHeight="1">
+    <row r="2" spans="1:28" ht="355" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -17891,52 +17930,56 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="F2" s="3">
         <v>2019</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="6">
+        <v>5</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="S2" s="8"/>
       <c r="T2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
@@ -17951,76 +17994,76 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="11">
         <v>13</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="F3" s="9">
         <v>2017</v>
       </c>
       <c r="G3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="L3" s="11">
         <v>16</v>
       </c>
       <c r="M3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="P3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="R3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="S3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="T3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="U3" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="V3" s="13"/>
       <c r="W3" s="13"/>
       <c r="X3" s="13"/>
       <c r="Y3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="AA3" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="AA3" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="AB3" s="13"/>
     </row>
@@ -18029,77 +18072,77 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="11">
         <v>13</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="F4" s="9">
         <v>2018</v>
       </c>
       <c r="G4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="K4" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="L4" s="11">
         <v>9</v>
       </c>
       <c r="M4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="O4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="P4" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="Q4" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="R4" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="S4" s="14"/>
       <c r="T4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
       <c r="X4" s="14"/>
       <c r="Y4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="Z4" s="12" t="s">
+      <c r="AA4" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AA4" s="12" t="s">
+      <c r="AB4" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="AB4" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="409.5" customHeight="1">
@@ -18107,83 +18150,83 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>64</v>
       </c>
       <c r="F5" s="9">
         <v>2018</v>
       </c>
       <c r="G5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="12" t="s">
+      <c r="K5" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="L5" s="11">
         <v>4</v>
       </c>
       <c r="M5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="O5" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="P5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="Q5" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="R5" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="S5" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="T5" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="U5" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="U5" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="V5" s="14"/>
       <c r="W5" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="X5" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="Y5" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="Y5" s="12" t="s">
+      <c r="Z5" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="Z5" s="12" t="s">
+      <c r="AA5" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="AA5" s="12" t="s">
+      <c r="AB5" s="16" t="s">
         <v>81</v>
-      </c>
-      <c r="AB5" s="16" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="409.5" customHeight="1">
@@ -18191,65 +18234,65 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>83</v>
+        <v>616</v>
       </c>
       <c r="C6" s="11">
         <v>4</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6" s="9">
         <v>2019</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="L6" s="11">
         <v>10</v>
       </c>
       <c r="M6" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="P6" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="Q6" s="14"/>
       <c r="R6" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="T6" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="U6" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="T6" s="10" t="s">
+      <c r="V6" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="U6" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="V6" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="W6" s="14"/>
       <c r="X6" s="14"/>
@@ -18263,61 +18306,65 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>98</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="F7" s="9">
         <v>2019</v>
       </c>
       <c r="G7" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="L7" s="14">
+        <v>12</v>
+      </c>
+      <c r="M7" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="N7" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="12" t="s">
+      <c r="O7" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="P7" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="Q7" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="R7" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>110</v>
       </c>
       <c r="S7" s="14"/>
       <c r="T7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="V7" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="U7" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="V7" s="12" t="s">
-        <v>113</v>
       </c>
       <c r="W7" s="14"/>
       <c r="X7" s="14"/>
@@ -18331,56 +18378,60 @@
         <v>9</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C8" s="9">
         <v>50</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F8" s="9">
         <v>2014</v>
       </c>
       <c r="G8" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18" t="s">
+      <c r="K8" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="L8" s="14">
+        <v>10</v>
+      </c>
+      <c r="M8" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="N8" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="12" t="s">
+      <c r="O8" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="P8" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>124</v>
       </c>
       <c r="Q8" s="14"/>
       <c r="R8" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S8" s="14"/>
       <c r="T8" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="V8" s="14"/>
       <c r="W8" s="14"/>
@@ -18395,60 +18446,64 @@
         <v>10</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="9">
         <v>30</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F9" s="9">
         <v>2016</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>625</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="10" t="s">
+      <c r="K9" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="L9" s="13">
+        <v>10</v>
+      </c>
+      <c r="M9" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="N9" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="10" t="s">
+      <c r="O9" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="P9" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="Q9" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="P9" s="12" t="s">
+      <c r="R9" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="Q9" s="12" t="s">
+      <c r="S9" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="R9" s="12" t="s">
+      <c r="T9" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="S9" s="12" t="s">
+      <c r="U9" s="12" t="s">
         <v>141</v>
-      </c>
-      <c r="T9" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="U9" s="12" t="s">
-        <v>143</v>
       </c>
       <c r="V9" s="14"/>
       <c r="W9" s="14"/>
@@ -18463,60 +18518,64 @@
         <v>13</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" s="11">
         <v>67</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F10" s="9">
         <v>2016</v>
       </c>
       <c r="G10" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="K10" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="10" t="s">
+      <c r="L10" s="13">
+        <v>11</v>
+      </c>
+      <c r="M10" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="K10" s="10" t="s">
+      <c r="N10" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="L10" s="13"/>
-      <c r="M10" s="10" t="s">
+      <c r="O10" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="P10" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="Q10" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="R10" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="S10" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="T10" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="R10" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="S10" s="12" t="s">
+      <c r="U10" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="T10" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="U10" s="12" t="s">
-        <v>157</v>
       </c>
       <c r="V10" s="14"/>
       <c r="W10" s="14"/>
@@ -18531,57 +18590,61 @@
         <v>14</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C11" s="11">
         <v>5</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F11" s="9">
         <v>2018</v>
       </c>
       <c r="G11" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="12" t="s">
+      <c r="K11" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="L11" s="14">
+        <v>2</v>
+      </c>
+      <c r="M11" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="N11" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="12" t="s">
+      <c r="O11" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="P11" s="12" t="s">
         <v>166</v>
-      </c>
-      <c r="O11" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>168</v>
       </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S11" s="14"/>
       <c r="T11" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="U11" s="14"/>
       <c r="V11" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="W11" s="14"/>
       <c r="X11" s="14"/>
@@ -18595,57 +18658,63 @@
         <v>15</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>171</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>173</v>
       </c>
       <c r="F12" s="9">
         <v>2019</v>
       </c>
       <c r="G12" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>626</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="10" t="s">
+      <c r="K12" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="L12" s="13">
+        <v>2</v>
+      </c>
+      <c r="M12" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="N12" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="10" t="s">
+      <c r="O12" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="N12" s="12" t="s">
+      <c r="P12" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="O12" s="12" t="s">
+      <c r="Q12" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="P12" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>182</v>
-      </c>
       <c r="R12" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
+      <c r="T12" s="14" t="s">
+        <v>633</v>
+      </c>
       <c r="U12" s="14"/>
       <c r="V12" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="W12" s="14"/>
       <c r="X12" s="14"/>
@@ -18659,60 +18728,64 @@
         <v>16</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C13" s="9">
         <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F13" s="9">
         <v>2017</v>
       </c>
       <c r="G13" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="J13" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="12" t="s">
+      <c r="K13" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="L13" s="14">
+        <v>8</v>
+      </c>
+      <c r="M13" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="N13" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="12" t="s">
+      <c r="O13" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="N13" s="12" t="s">
+      <c r="P13" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="O13" s="12" t="s">
+      <c r="Q13" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="P13" s="12" t="s">
+      <c r="R13" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="Q13" s="12" t="s">
+      <c r="S13" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="R13" s="12" t="s">
+      <c r="T13" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="S13" s="12" t="s">
+      <c r="U13" s="12" t="s">
         <v>196</v>
-      </c>
-      <c r="T13" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="U13" s="12" t="s">
-        <v>198</v>
       </c>
       <c r="V13" s="14"/>
       <c r="W13" s="14"/>
@@ -18727,56 +18800,60 @@
         <v>17</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C14" s="20">
         <v>12</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F14" s="9">
         <v>2016</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>627</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="J14" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="10" t="s">
+      <c r="K14" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="L14" s="13">
+        <v>3</v>
+      </c>
+      <c r="M14" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="N14" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="L14" s="13"/>
-      <c r="M14" s="10" t="s">
+      <c r="O14" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="P14" s="12" t="s">
         <v>207</v>
-      </c>
-      <c r="O14" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="P14" s="12" t="s">
-        <v>209</v>
       </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S14" s="14"/>
       <c r="T14" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="U14" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="V14" s="14"/>
       <c r="W14" s="14"/>
@@ -18786,33 +18863,55 @@
       <c r="AA14" s="14"/>
       <c r="AB14" s="14"/>
     </row>
-    <row r="15" spans="1:28" ht="22" customHeight="1">
+    <row r="15" spans="1:28" ht="238" customHeight="1">
       <c r="A15" s="9">
         <v>20</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
+      <c r="B15" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>635</v>
+      </c>
       <c r="D15" s="22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="F15" s="23">
+        <v>2019</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="L15" s="14">
+        <v>8</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>632</v>
+      </c>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
       <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
+      <c r="T15" s="14" t="s">
+        <v>634</v>
+      </c>
       <c r="U15" s="14"/>
       <c r="V15" s="14"/>
       <c r="W15" s="14"/>
@@ -18827,60 +18926,64 @@
         <v>21</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C16" s="25">
         <v>36</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F16" s="9">
         <v>2015</v>
       </c>
       <c r="G16" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="J16" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="12" t="s">
+      <c r="K16" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="L16" s="13">
+        <v>10</v>
+      </c>
+      <c r="M16" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="N16" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="L16" s="13"/>
-      <c r="M16" s="10" t="s">
+      <c r="O16" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="P16" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="O16" s="12" t="s">
+      <c r="Q16" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="P16" s="12" t="s">
+      <c r="R16" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="S16" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="Q16" s="12" t="s">
+      <c r="T16" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="R16" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="S16" s="12" t="s">
+      <c r="U16" s="12" t="s">
         <v>226</v>
-      </c>
-      <c r="T16" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="U16" s="12" t="s">
-        <v>228</v>
       </c>
       <c r="V16" s="14"/>
       <c r="W16" s="14"/>
@@ -18895,60 +18998,64 @@
         <v>22</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C17" s="9">
         <v>75</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F17" s="9">
         <v>2014</v>
       </c>
       <c r="G17" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="J17" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="12" t="s">
+      <c r="K17" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="L17" s="14">
+        <v>8</v>
+      </c>
+      <c r="M17" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="N17" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="L17" s="14"/>
-      <c r="M17" s="12" t="s">
+      <c r="O17" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="N17" s="12" t="s">
+      <c r="P17" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="O17" s="12" t="s">
+      <c r="Q17" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="P17" s="12" t="s">
+      <c r="R17" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="Q17" s="12" t="s">
+      <c r="S17" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="R17" s="12" t="s">
+      <c r="T17" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="S17" s="12" t="s">
+      <c r="U17" s="12" t="s">
         <v>242</v>
-      </c>
-      <c r="T17" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="U17" s="12" t="s">
-        <v>244</v>
       </c>
       <c r="V17" s="14"/>
       <c r="W17" s="14"/>
@@ -18963,60 +19070,64 @@
         <v>27</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C18" s="11">
         <v>9</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F18" s="9">
         <v>2016</v>
       </c>
       <c r="G18" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="12" t="s">
+      <c r="L18" s="14">
+        <v>8</v>
+      </c>
+      <c r="M18" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="K18" s="10" t="s">
+      <c r="N18" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="L18" s="14"/>
-      <c r="M18" s="12" t="s">
+      <c r="O18" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="N18" s="12" t="s">
+      <c r="P18" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="O18" s="12" t="s">
+      <c r="Q18" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="P18" s="12" t="s">
+      <c r="R18" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="Q18" s="12" t="s">
+      <c r="S18" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="R18" s="12" t="s">
+      <c r="T18" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="S18" s="12" t="s">
+      <c r="U18" s="12" t="s">
         <v>255</v>
-      </c>
-      <c r="T18" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="U18" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="V18" s="14"/>
       <c r="W18" s="14"/>
@@ -19031,58 +19142,64 @@
         <v>30</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C19" s="9">
         <v>13</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F19" s="9">
         <v>2018</v>
       </c>
       <c r="G19" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>633</v>
+      </c>
+      <c r="L19" s="14">
+        <v>16</v>
+      </c>
+      <c r="M19" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="12" t="s">
+      <c r="N19" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="J19" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="12" t="s">
+      <c r="O19" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="N19" s="12" t="s">
+      <c r="P19" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="O19" s="12" t="s">
+      <c r="Q19" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="R19" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="Q19" s="12" t="s">
+      <c r="S19" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="R19" s="12" t="s">
+      <c r="T19" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="S19" s="10" t="s">
+      <c r="U19" s="12" t="s">
         <v>269</v>
-      </c>
-      <c r="T19" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="U19" s="12" t="s">
-        <v>271</v>
       </c>
       <c r="V19" s="14"/>
       <c r="W19" s="14"/>
@@ -19097,58 +19214,64 @@
         <v>38</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C20" s="9">
         <v>3</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F20" s="9">
         <v>2016</v>
       </c>
       <c r="G20" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="J20" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="12" t="s">
+      <c r="K20" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="L20" s="14">
+        <v>4</v>
+      </c>
+      <c r="M20" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="N20" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="12" t="s">
+      <c r="O20" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="N20" s="12" t="s">
+      <c r="P20" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="O20" s="12" t="s">
+      <c r="Q20" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="P20" s="10" t="s">
+      <c r="R20" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="Q20" s="12" t="s">
+      <c r="S20" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="R20" s="12" t="s">
+      <c r="T20" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="S20" s="12" t="s">
+      <c r="U20" s="12" t="s">
         <v>284</v>
-      </c>
-      <c r="T20" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="U20" s="12" t="s">
-        <v>286</v>
       </c>
       <c r="V20" s="14"/>
       <c r="W20" s="14"/>
@@ -19163,58 +19286,64 @@
         <v>48</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C21" s="9">
+        <v>108</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>287</v>
-      </c>
-      <c r="C21" s="9">
-        <v>96</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>289</v>
       </c>
       <c r="F21" s="9">
         <v>2015</v>
       </c>
       <c r="G21" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="J21" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="12" t="s">
+      <c r="K21" s="14" t="s">
+        <v>638</v>
+      </c>
+      <c r="L21" s="14">
+        <v>10</v>
+      </c>
+      <c r="M21" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="N21" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="12" t="s">
+      <c r="O21" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="N21" s="12" t="s">
+      <c r="P21" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="O21" s="10" t="s">
+      <c r="Q21" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="P21" s="12" t="s">
+      <c r="R21" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="Q21" s="12" t="s">
+      <c r="S21" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="R21" s="12" t="s">
+      <c r="T21" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="S21" s="10" t="s">
+      <c r="U21" s="12" t="s">
         <v>299</v>
-      </c>
-      <c r="T21" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="U21" s="12" t="s">
-        <v>301</v>
       </c>
       <c r="V21" s="14"/>
       <c r="W21" s="14"/>
@@ -19229,53 +19358,57 @@
         <v>47</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C22" s="9">
         <v>21</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F22" s="9">
         <v>2015</v>
       </c>
       <c r="G22" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="12" t="s">
+      <c r="L22" s="14">
+        <v>8</v>
+      </c>
+      <c r="M22" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="J22" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K22" s="12" t="s">
+      <c r="N22" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="L22" s="14"/>
-      <c r="M22" s="12" t="s">
+      <c r="O22" s="12" t="s">
         <v>307</v>
       </c>
-      <c r="N22" s="12" t="s">
+      <c r="P22" s="12" t="s">
         <v>308</v>
-      </c>
-      <c r="O22" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="P22" s="12" t="s">
-        <v>310</v>
       </c>
       <c r="Q22" s="14"/>
       <c r="R22" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="S22" s="14"/>
       <c r="T22" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="U22" s="14"/>
       <c r="V22" s="14"/>
@@ -19291,52 +19424,56 @@
         <v>20</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>313</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>315</v>
       </c>
       <c r="F23" s="9">
         <v>2019</v>
       </c>
       <c r="G23" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="K23" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="12" t="s">
+      <c r="L23" s="14">
+        <v>8</v>
+      </c>
+      <c r="M23" s="12" t="s">
         <v>317</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="L23" s="14"/>
-      <c r="M23" s="12" t="s">
-        <v>319</v>
       </c>
       <c r="N23" s="14"/>
       <c r="O23" s="14"/>
       <c r="P23" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="Q23" s="14"/>
       <c r="R23" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="S23" s="14"/>
       <c r="T23" s="10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="U23" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="V23" s="14"/>
       <c r="W23" s="14"/>
@@ -19351,54 +19488,58 @@
         <v>33</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C24" s="9">
         <v>137</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F24" s="9">
         <v>2012</v>
       </c>
       <c r="G24" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="K24" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="18" t="s">
+      <c r="L24" s="14">
+        <v>10</v>
+      </c>
+      <c r="M24" s="12" t="s">
         <v>328</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="L24" s="14"/>
-      <c r="M24" s="12" t="s">
-        <v>330</v>
       </c>
       <c r="N24" s="14"/>
       <c r="O24" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
       <c r="S24" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="T24" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="U24" s="12" t="s">
         <v>333</v>
-      </c>
-      <c r="T24" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="U24" s="12" t="s">
-        <v>335</v>
       </c>
       <c r="V24" s="14"/>
       <c r="W24" s="14"/>
@@ -19413,60 +19554,64 @@
         <v>26</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F25" s="9">
         <v>2019</v>
       </c>
       <c r="G25" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="K25" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="10" t="s">
+      <c r="L25" s="14">
+        <v>2</v>
+      </c>
+      <c r="M25" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="J25" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="K25" s="10" t="s">
+      <c r="N25" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="L25" s="14"/>
-      <c r="M25" s="12" t="s">
+      <c r="O25" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="N25" s="12" t="s">
+      <c r="P25" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="O25" s="12" t="s">
+      <c r="Q25" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="P25" s="12" t="s">
+      <c r="R25" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="S25" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="Q25" s="12" t="s">
+      <c r="T25" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="R25" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="S25" s="12" t="s">
+      <c r="U25" s="12" t="s">
         <v>346</v>
-      </c>
-      <c r="T25" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="U25" s="12" t="s">
-        <v>348</v>
       </c>
       <c r="V25" s="14"/>
       <c r="W25" s="14"/>
@@ -19481,54 +19626,58 @@
         <v>28</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="9">
         <v>5</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F26" s="9">
         <v>2018</v>
       </c>
       <c r="G26" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="K26" s="30" t="s">
         <v>351</v>
       </c>
-      <c r="H26" s="28"/>
-      <c r="I26" s="29" t="s">
+      <c r="L26" s="13">
+        <v>4</v>
+      </c>
+      <c r="M26" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="J26" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="K26" s="30" t="s">
+      <c r="N26" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="L26" s="13"/>
-      <c r="M26" s="10" t="s">
+      <c r="O26" s="12" t="s">
         <v>354</v>
-      </c>
-      <c r="N26" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="O26" s="12" t="s">
-        <v>356</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
       <c r="R26" s="12" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="S26" s="14"/>
       <c r="T26" s="16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="U26" s="12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="V26" s="14"/>
       <c r="W26" s="14"/>
@@ -19543,60 +19692,64 @@
         <v>31</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C27" s="9">
         <v>17</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F27" s="9">
         <v>2015</v>
       </c>
       <c r="G27" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>628</v>
+      </c>
+      <c r="I27" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="K27" s="30" t="s">
         <v>363</v>
       </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="29" t="s">
+      <c r="L27" s="13">
+        <v>8</v>
+      </c>
+      <c r="M27" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="K27" s="30" t="s">
+      <c r="N27" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="L27" s="13"/>
-      <c r="M27" s="10" t="s">
+      <c r="O27" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="N27" s="12" t="s">
+      <c r="P27" s="12" t="s">
         <v>367</v>
       </c>
-      <c r="O27" s="12" t="s">
+      <c r="Q27" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="P27" s="12" t="s">
+      <c r="R27" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="Q27" s="12" t="s">
+      <c r="S27" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="T27" s="16" t="s">
         <v>370</v>
       </c>
-      <c r="R27" s="12" t="s">
+      <c r="U27" s="12" t="s">
         <v>371</v>
-      </c>
-      <c r="S27" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="T27" s="16" t="s">
-        <v>372</v>
-      </c>
-      <c r="U27" s="12" t="s">
-        <v>373</v>
       </c>
       <c r="V27" s="14"/>
       <c r="W27" s="14"/>
@@ -19611,49 +19764,53 @@
         <v>44</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C28" s="9">
         <v>23</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F28" s="9">
         <v>2016</v>
       </c>
       <c r="G28" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="K28" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="H28" s="13"/>
-      <c r="I28" s="10" t="s">
+      <c r="L28" s="13">
+        <v>4</v>
+      </c>
+      <c r="M28" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="J28" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="K28" s="10" t="s">
+      <c r="N28" s="12" t="s">
         <v>377</v>
       </c>
-      <c r="L28" s="13"/>
-      <c r="M28" s="10" t="s">
+      <c r="O28" s="12" t="s">
         <v>378</v>
-      </c>
-      <c r="N28" s="12" t="s">
-        <v>379</v>
-      </c>
-      <c r="O28" s="12" t="s">
-        <v>380</v>
       </c>
       <c r="P28" s="14"/>
       <c r="Q28" s="14"/>
       <c r="R28" s="14"/>
       <c r="S28" s="14"/>
       <c r="T28" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="U28" s="14"/>
       <c r="V28" s="14"/>
@@ -19668,47 +19825,57 @@
       <c r="A29" s="9">
         <v>43</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="B29" s="13" t="s">
+        <v>619</v>
+      </c>
+      <c r="C29" s="14">
+        <v>35</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>618</v>
+      </c>
       <c r="E29" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F29" s="32">
         <v>2016</v>
       </c>
       <c r="G29" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>382</v>
+      </c>
+      <c r="J29" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="H29" s="28"/>
-      <c r="I29" s="29" t="s">
+      <c r="K29" s="30" t="s">
         <v>384</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="L29" s="13">
+        <v>13</v>
+      </c>
+      <c r="M29" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="K29" s="30" t="s">
+      <c r="N29" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="L29" s="13"/>
-      <c r="M29" s="10" t="s">
+      <c r="O29" s="12" t="s">
         <v>387</v>
-      </c>
-      <c r="N29" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="O29" s="12" t="s">
-        <v>389</v>
       </c>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
       <c r="R29" s="14"/>
       <c r="S29" s="14"/>
       <c r="T29" s="16" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="U29" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="V29" s="14"/>
       <c r="W29" s="14"/>
@@ -19723,56 +19890,60 @@
         <v>51</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C30" s="9">
         <v>3</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F30" s="9">
         <v>2019</v>
       </c>
       <c r="G30" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="J30" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="H30" s="13"/>
-      <c r="I30" s="10" t="s">
+      <c r="K30" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="L30" s="13">
+        <v>11</v>
+      </c>
+      <c r="M30" s="10" t="s">
         <v>397</v>
-      </c>
-      <c r="K30" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="L30" s="13"/>
-      <c r="M30" s="10" t="s">
-        <v>399</v>
       </c>
       <c r="N30" s="14"/>
       <c r="O30" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="P30" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q30" s="12" t="s">
         <v>400</v>
       </c>
-      <c r="P30" s="12" t="s">
+      <c r="R30" s="12" t="s">
         <v>401</v>
-      </c>
-      <c r="Q30" s="12" t="s">
-        <v>402</v>
-      </c>
-      <c r="R30" s="12" t="s">
-        <v>403</v>
       </c>
       <c r="S30" s="14"/>
       <c r="T30" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="U30" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="V30" s="14"/>
       <c r="W30" s="14"/>
@@ -19787,56 +19958,60 @@
         <v>52</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C31" s="9">
         <v>3</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F31" s="9">
         <v>2019</v>
       </c>
       <c r="G31" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="K31" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="H31" s="13"/>
-      <c r="I31" s="10" t="s">
+      <c r="L31" s="13">
+        <v>8</v>
+      </c>
+      <c r="M31" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="J31" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="K31" s="10" t="s">
+      <c r="N31" s="12" t="s">
         <v>411</v>
       </c>
-      <c r="L31" s="13"/>
-      <c r="M31" s="10" t="s">
+      <c r="O31" s="12" t="s">
         <v>412</v>
       </c>
-      <c r="N31" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="O31" s="12" t="s">
-        <v>414</v>
-      </c>
       <c r="P31" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="Q31" s="14"/>
       <c r="R31" s="12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="S31" s="14"/>
       <c r="T31" s="10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="U31" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="V31" s="14"/>
       <c r="W31" s="14"/>
@@ -19851,54 +20026,58 @@
         <v>63</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C32" s="9">
         <v>4</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F32" s="9">
         <v>2019</v>
       </c>
       <c r="G32" s="35" t="s">
+        <v>419</v>
+      </c>
+      <c r="H32" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="37" t="s">
+        <v>420</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="K32" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37" t="s">
+      <c r="L32" s="13">
+        <v>31</v>
+      </c>
+      <c r="M32" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="J32" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="K32" s="10" t="s">
+      <c r="N32" s="12" t="s">
         <v>423</v>
       </c>
-      <c r="L32" s="13"/>
-      <c r="M32" s="10" t="s">
+      <c r="O32" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="N32" s="12" t="s">
+      <c r="P32" s="12" t="s">
         <v>425</v>
-      </c>
-      <c r="O32" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="P32" s="12" t="s">
-        <v>427</v>
       </c>
       <c r="Q32" s="14"/>
       <c r="R32" s="14"/>
       <c r="S32" s="14"/>
       <c r="T32" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="U32" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="V32" s="14"/>
       <c r="W32" s="14"/>
@@ -19913,56 +20092,60 @@
         <v>73</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C33" s="9">
         <v>8</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F33" s="9">
         <v>2018</v>
       </c>
       <c r="G33" s="30" t="s">
+        <v>431</v>
+      </c>
+      <c r="H33" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="I33" s="37" t="s">
+        <v>432</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="K33" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37" t="s">
+      <c r="L33" s="13">
+        <v>5</v>
+      </c>
+      <c r="M33" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="J33" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="K33" s="10" t="s">
+      <c r="N33" s="12" t="s">
         <v>435</v>
-      </c>
-      <c r="L33" s="13"/>
-      <c r="M33" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="N33" s="12" t="s">
-        <v>437</v>
       </c>
       <c r="O33" s="14"/>
       <c r="P33" s="12" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="Q33" s="14"/>
       <c r="R33" s="12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="S33" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="T33" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="U33" s="12" t="s">
         <v>439</v>
-      </c>
-      <c r="T33" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="U33" s="12" t="s">
-        <v>441</v>
       </c>
       <c r="V33" s="14"/>
       <c r="W33" s="14"/>
@@ -19977,58 +20160,62 @@
         <v>69</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>442</v>
+        <v>620</v>
       </c>
       <c r="C34" s="9">
         <v>21</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E34" s="38" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F34" s="9">
         <v>2017</v>
       </c>
       <c r="G34" s="16" t="s">
+        <v>442</v>
+      </c>
+      <c r="H34" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="37" t="s">
+        <v>443</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="L34" s="13">
+        <v>11</v>
+      </c>
+      <c r="M34" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37" t="s">
+      <c r="N34" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="J34" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="K34" s="16" t="s">
+      <c r="O34" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="L34" s="13"/>
-      <c r="M34" s="10" t="s">
+      <c r="P34" s="12" t="s">
         <v>448</v>
-      </c>
-      <c r="N34" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="O34" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="P34" s="12" t="s">
-        <v>451</v>
       </c>
       <c r="Q34" s="14"/>
       <c r="R34" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="S34" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="T34" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="U34" s="12" t="s">
         <v>452</v>
-      </c>
-      <c r="S34" s="12" t="s">
-        <v>453</v>
-      </c>
-      <c r="T34" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="U34" s="12" t="s">
-        <v>455</v>
       </c>
       <c r="V34" s="14"/>
       <c r="W34" s="14"/>
@@ -20043,52 +20230,56 @@
         <v>67</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C35" s="9">
         <v>28</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E35" s="34" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="F35" s="9">
         <v>2016</v>
       </c>
       <c r="G35" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="H35" s="36" t="s">
+        <v>628</v>
+      </c>
+      <c r="I35" s="37" t="s">
+        <v>457</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="L35" s="13">
+        <v>8</v>
+      </c>
+      <c r="M35" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37" t="s">
+      <c r="N35" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="J35" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="K35" s="16" t="s">
+      <c r="O35" s="12" t="s">
         <v>461</v>
-      </c>
-      <c r="L35" s="13"/>
-      <c r="M35" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="N35" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="O35" s="12" t="s">
-        <v>464</v>
       </c>
       <c r="P35" s="14"/>
       <c r="Q35" s="14"/>
       <c r="R35" s="14"/>
       <c r="S35" s="14"/>
       <c r="T35" s="16" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="U35" s="16" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="V35" s="14"/>
       <c r="W35" s="14"/>
@@ -20103,52 +20294,56 @@
         <v>66</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C36" s="9">
         <v>12</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E36" s="40" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="F36" s="9">
         <v>2016</v>
       </c>
       <c r="G36" s="39" t="s">
+        <v>467</v>
+      </c>
+      <c r="H36" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="I36" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="L36" s="13">
+        <v>8</v>
+      </c>
+      <c r="M36" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37" t="s">
+      <c r="N36" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="J36" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="K36" s="16" t="s">
+      <c r="O36" s="12" t="s">
         <v>472</v>
-      </c>
-      <c r="L36" s="13"/>
-      <c r="M36" s="10" t="s">
-        <v>473</v>
-      </c>
-      <c r="N36" s="12" t="s">
-        <v>474</v>
-      </c>
-      <c r="O36" s="12" t="s">
-        <v>475</v>
       </c>
       <c r="P36" s="14"/>
       <c r="Q36" s="14"/>
       <c r="R36" s="14"/>
       <c r="S36" s="14"/>
       <c r="T36" s="16" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="U36" s="16" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="V36" s="14"/>
       <c r="W36" s="14"/>
@@ -20163,57 +20358,61 @@
         <v>96</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C37" s="9">
         <v>0</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E37" s="40" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F37" s="9">
         <v>2017</v>
       </c>
       <c r="G37" s="16" t="s">
+        <v>478</v>
+      </c>
+      <c r="H37" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="I37" s="37" t="s">
+        <v>629</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="K37" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="L37" s="41">
+        <v>10</v>
+      </c>
+      <c r="M37" s="16" t="s">
         <v>481</v>
       </c>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37" t="s">
+      <c r="N37" s="12" t="s">
         <v>482</v>
       </c>
-      <c r="J37" s="12" t="s">
+      <c r="O37" s="12" t="s">
         <v>483</v>
       </c>
-      <c r="K37" s="16" t="s">
+      <c r="P37" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="L37" s="41"/>
-      <c r="M37" s="16" t="s">
+      <c r="Q37" s="12" t="s">
         <v>485</v>
       </c>
-      <c r="N37" s="12" t="s">
+      <c r="R37" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="S37" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="T37" s="16" t="s">
         <v>486</v>
-      </c>
-      <c r="O37" s="12" t="s">
-        <v>487</v>
-      </c>
-      <c r="P37" s="12" t="s">
-        <v>488</v>
-      </c>
-      <c r="Q37" s="12" t="s">
-        <v>489</v>
-      </c>
-      <c r="R37" s="12" t="s">
-        <v>488</v>
-      </c>
-      <c r="S37" s="12" t="s">
-        <v>488</v>
-      </c>
-      <c r="T37" s="16" t="s">
-        <v>490</v>
       </c>
       <c r="U37" s="41"/>
       <c r="V37" s="14"/>
@@ -20229,49 +20428,53 @@
         <v>35</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C38" s="9">
         <v>65</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>492</v>
+        <v>623</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="F38" s="9">
         <v>2015</v>
       </c>
       <c r="G38" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="H38" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="K38" s="42" t="s">
+        <v>491</v>
+      </c>
+      <c r="L38" s="41">
+        <v>17</v>
+      </c>
+      <c r="M38" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="O38" s="12" t="s">
         <v>494</v>
-      </c>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37" t="s">
-        <v>495</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="K38" s="42" t="s">
-        <v>496</v>
-      </c>
-      <c r="L38" s="41"/>
-      <c r="M38" s="16" t="s">
-        <v>497</v>
-      </c>
-      <c r="N38" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="O38" s="12" t="s">
-        <v>499</v>
       </c>
       <c r="P38" s="14"/>
       <c r="Q38" s="14"/>
       <c r="R38" s="14"/>
       <c r="S38" s="14"/>
       <c r="T38" s="16" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="U38" s="41"/>
       <c r="V38" s="14"/>
@@ -20287,39 +20490,43 @@
         <v>24</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="C39" s="9">
         <v>15</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="E39" s="43" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="F39" s="9">
         <v>2018</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>504</v>
-      </c>
-      <c r="H39" s="44"/>
-      <c r="I39" s="45" t="s">
-        <v>505</v>
+        <v>499</v>
+      </c>
+      <c r="H39" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="I39" s="44" t="s">
+        <v>500</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K39" s="42" t="s">
-        <v>506</v>
-      </c>
-      <c r="L39" s="41"/>
+        <v>501</v>
+      </c>
+      <c r="L39" s="41">
+        <v>27</v>
+      </c>
       <c r="M39" s="16" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="O39" s="14"/>
       <c r="P39" s="14"/>
@@ -20327,7 +20534,7 @@
       <c r="R39" s="14"/>
       <c r="S39" s="14"/>
       <c r="T39" s="16" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="U39" s="41"/>
       <c r="V39" s="14"/>
@@ -20343,39 +20550,43 @@
         <v>77</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="C40" s="9">
         <v>9</v>
       </c>
       <c r="D40" s="33" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="F40" s="9">
         <v>2019</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>513</v>
-      </c>
-      <c r="H40" s="28"/>
+        <v>508</v>
+      </c>
+      <c r="H40" s="28" t="s">
+        <v>44</v>
+      </c>
       <c r="I40" s="29" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K40" s="42" t="s">
-        <v>515</v>
-      </c>
-      <c r="L40" s="41"/>
+        <v>510</v>
+      </c>
+      <c r="L40" s="41">
+        <v>11</v>
+      </c>
       <c r="M40" s="16" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="O40" s="14"/>
       <c r="P40" s="14"/>
@@ -20383,7 +20594,7 @@
       <c r="R40" s="14"/>
       <c r="S40" s="14"/>
       <c r="T40" s="16" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="U40" s="41"/>
       <c r="V40" s="14"/>
@@ -20399,33 +20610,43 @@
         <v>78</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="46"/>
+        <v>514</v>
+      </c>
+      <c r="C41" s="14">
+        <v>12</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>624</v>
+      </c>
       <c r="E41" s="31" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="F41" s="9">
         <v>2017</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>521</v>
-      </c>
-      <c r="H41" s="28"/>
+        <v>516</v>
+      </c>
+      <c r="H41" s="28" t="s">
+        <v>44</v>
+      </c>
       <c r="I41" s="29" t="s">
-        <v>522</v>
-      </c>
-      <c r="J41" s="14"/>
+        <v>517</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>131</v>
+      </c>
       <c r="K41" s="16" t="s">
-        <v>523</v>
-      </c>
-      <c r="L41" s="41"/>
+        <v>518</v>
+      </c>
+      <c r="L41" s="41">
+        <v>5</v>
+      </c>
       <c r="M41" s="16" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="O41" s="14"/>
       <c r="P41" s="14"/>
@@ -20433,7 +20654,7 @@
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
       <c r="T41" s="16" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="U41" s="41"/>
       <c r="V41" s="14"/>
@@ -20449,47 +20670,53 @@
         <v>81</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>527</v>
-      </c>
-      <c r="C42" s="14"/>
+        <v>617</v>
+      </c>
+      <c r="C42" s="14">
+        <v>105</v>
+      </c>
       <c r="D42" s="16" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="F42" s="9">
         <v>2012</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>530</v>
-      </c>
-      <c r="H42" s="28"/>
+        <v>524</v>
+      </c>
+      <c r="H42" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="I42" s="29" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K42" s="16" t="s">
-        <v>532</v>
-      </c>
-      <c r="L42" s="41"/>
+        <v>526</v>
+      </c>
+      <c r="L42" s="41">
+        <v>9</v>
+      </c>
       <c r="M42" s="16" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="O42" s="12" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="P42" s="14"/>
       <c r="Q42" s="14"/>
       <c r="R42" s="14"/>
       <c r="S42" s="14"/>
       <c r="T42" s="16" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="U42" s="41"/>
       <c r="V42" s="14"/>
@@ -20505,49 +20732,55 @@
         <v>82</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>527</v>
-      </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="47" t="s">
-        <v>528</v>
-      </c>
-      <c r="E43" s="48" t="s">
-        <v>536</v>
+        <v>617</v>
+      </c>
+      <c r="C43" s="14">
+        <v>103</v>
+      </c>
+      <c r="D43" s="46" t="s">
+        <v>522</v>
+      </c>
+      <c r="E43" s="47" t="s">
+        <v>530</v>
       </c>
       <c r="F43" s="9">
         <v>2012</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>537</v>
-      </c>
-      <c r="H43" s="41"/>
+        <v>531</v>
+      </c>
+      <c r="H43" s="41" t="s">
+        <v>628</v>
+      </c>
       <c r="I43" s="16" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K43" s="16" t="s">
-        <v>539</v>
-      </c>
-      <c r="L43" s="41"/>
+        <v>533</v>
+      </c>
+      <c r="L43" s="41">
+        <v>5</v>
+      </c>
       <c r="M43" s="16" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="N43" s="12" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="O43" s="12" t="s">
-        <v>487</v>
-      </c>
-      <c r="P43" s="49"/>
+        <v>483</v>
+      </c>
+      <c r="P43" s="48"/>
       <c r="Q43" s="14"/>
       <c r="R43" s="14"/>
       <c r="S43" s="12" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="T43" s="16" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="U43" s="41"/>
       <c r="V43" s="14"/>
@@ -20563,45 +20796,53 @@
         <v>85</v>
       </c>
       <c r="B44" s="10" t="s">
+        <v>538</v>
+      </c>
+      <c r="C44" s="14">
+        <v>1</v>
+      </c>
+      <c r="D44" s="49" t="s">
+        <v>539</v>
+      </c>
+      <c r="E44" s="50" t="s">
+        <v>540</v>
+      </c>
+      <c r="F44" s="51">
+        <v>2018</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>541</v>
+      </c>
+      <c r="H44" s="41" t="s">
+        <v>630</v>
+      </c>
+      <c r="I44" s="16" t="s">
+        <v>542</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="K44" s="41" t="s">
+        <v>637</v>
+      </c>
+      <c r="L44" s="41">
+        <v>13</v>
+      </c>
+      <c r="M44" s="16" t="s">
         <v>544</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="50" t="s">
+      <c r="N44" s="12" t="s">
         <v>545</v>
       </c>
-      <c r="E44" s="51" t="s">
-        <v>546</v>
-      </c>
-      <c r="F44" s="52">
-        <v>2018</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>547</v>
-      </c>
-      <c r="H44" s="41"/>
-      <c r="I44" s="16" t="s">
-        <v>548</v>
-      </c>
-      <c r="J44" s="12" t="s">
-        <v>549</v>
-      </c>
-      <c r="K44" s="41"/>
-      <c r="L44" s="41"/>
-      <c r="M44" s="16" t="s">
-        <v>550</v>
-      </c>
-      <c r="N44" s="12" t="s">
-        <v>551</v>
-      </c>
       <c r="O44" s="12" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="P44" s="14"/>
       <c r="Q44" s="14"/>
       <c r="R44" s="14"/>
       <c r="S44" s="14"/>
       <c r="T44" s="16" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="U44" s="41"/>
       <c r="V44" s="14"/>
@@ -20617,51 +20858,57 @@
         <v>88</v>
       </c>
       <c r="B45" s="10" t="s">
+        <v>547</v>
+      </c>
+      <c r="C45" s="14">
+        <v>2</v>
+      </c>
+      <c r="D45" s="52" t="s">
+        <v>548</v>
+      </c>
+      <c r="E45" s="53" t="s">
+        <v>549</v>
+      </c>
+      <c r="F45" s="51">
+        <v>2019</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="H45" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="I45" s="16" t="s">
+        <v>551</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="K45" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="L45" s="41">
+        <v>5</v>
+      </c>
+      <c r="M45" s="16" t="s">
         <v>553</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="53" t="s">
+      <c r="N45" s="12" t="s">
         <v>554</v>
       </c>
-      <c r="E45" s="54" t="s">
+      <c r="O45" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="P45" s="12" t="s">
         <v>555</v>
-      </c>
-      <c r="F45" s="52">
-        <v>2019</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>556</v>
-      </c>
-      <c r="H45" s="41"/>
-      <c r="I45" s="16" t="s">
-        <v>557</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="K45" s="16" t="s">
-        <v>558</v>
-      </c>
-      <c r="L45" s="41"/>
-      <c r="M45" s="16" t="s">
-        <v>559</v>
-      </c>
-      <c r="N45" s="12" t="s">
-        <v>560</v>
-      </c>
-      <c r="O45" s="12" t="s">
-        <v>487</v>
-      </c>
-      <c r="P45" s="12" t="s">
-        <v>561</v>
       </c>
       <c r="Q45" s="14"/>
       <c r="R45" s="12" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="S45" s="14"/>
-      <c r="T45" s="55" t="s">
-        <v>563</v>
+      <c r="T45" s="54" t="s">
+        <v>557</v>
       </c>
       <c r="U45" s="41"/>
       <c r="V45" s="14"/>
@@ -20677,49 +20924,55 @@
         <v>90</v>
       </c>
       <c r="B46" s="10" t="s">
+        <v>558</v>
+      </c>
+      <c r="C46" s="14">
+        <v>6</v>
+      </c>
+      <c r="D46" s="52" t="s">
+        <v>559</v>
+      </c>
+      <c r="E46" s="53" t="s">
+        <v>560</v>
+      </c>
+      <c r="F46" s="51">
+        <v>2019</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>561</v>
+      </c>
+      <c r="H46" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="I46" s="16" t="s">
+        <v>562</v>
+      </c>
+      <c r="J46" s="12" t="s">
+        <v>563</v>
+      </c>
+      <c r="K46" s="16" t="s">
         <v>564</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="53" t="s">
+      <c r="L46" s="41">
+        <v>10</v>
+      </c>
+      <c r="M46" s="16" t="s">
         <v>565</v>
       </c>
-      <c r="E46" s="54" t="s">
+      <c r="N46" s="12" t="s">
         <v>566</v>
       </c>
-      <c r="F46" s="52">
-        <v>2019</v>
-      </c>
-      <c r="G46" s="16" t="s">
-        <v>567</v>
-      </c>
-      <c r="H46" s="41"/>
-      <c r="I46" s="16" t="s">
-        <v>568</v>
-      </c>
-      <c r="J46" s="12" t="s">
-        <v>569</v>
-      </c>
-      <c r="K46" s="16" t="s">
-        <v>570</v>
-      </c>
-      <c r="L46" s="41"/>
-      <c r="M46" s="16" t="s">
-        <v>571</v>
-      </c>
-      <c r="N46" s="12" t="s">
-        <v>572</v>
-      </c>
       <c r="O46" s="12" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="P46" s="14"/>
       <c r="Q46" s="14"/>
       <c r="R46" s="12" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="S46" s="14"/>
       <c r="T46" s="16" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="U46" s="41"/>
       <c r="V46" s="14"/>
@@ -20735,49 +20988,55 @@
         <v>91</v>
       </c>
       <c r="B47" s="10" t="s">
+        <v>569</v>
+      </c>
+      <c r="C47" s="14">
+        <v>10</v>
+      </c>
+      <c r="D47" s="52" t="s">
+        <v>570</v>
+      </c>
+      <c r="E47" s="55" t="s">
+        <v>571</v>
+      </c>
+      <c r="F47" s="51">
+        <v>2018</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="H47" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="K47" s="16" t="s">
+        <v>573</v>
+      </c>
+      <c r="L47" s="41">
+        <v>9</v>
+      </c>
+      <c r="M47" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="N47" s="12" t="s">
         <v>575</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="53" t="s">
+      <c r="O47" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="P47" s="12" t="s">
         <v>576</v>
-      </c>
-      <c r="E47" s="56" t="s">
-        <v>577</v>
-      </c>
-      <c r="F47" s="52">
-        <v>2018</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>578</v>
-      </c>
-      <c r="H47" s="41"/>
-      <c r="I47" s="16" t="s">
-        <v>434</v>
-      </c>
-      <c r="J47" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="K47" s="16" t="s">
-        <v>579</v>
-      </c>
-      <c r="L47" s="41"/>
-      <c r="M47" s="16" t="s">
-        <v>580</v>
-      </c>
-      <c r="N47" s="12" t="s">
-        <v>581</v>
-      </c>
-      <c r="O47" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="P47" s="12" t="s">
-        <v>582</v>
       </c>
       <c r="Q47" s="14"/>
       <c r="R47" s="14"/>
       <c r="S47" s="14"/>
       <c r="T47" s="16" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="U47" s="41"/>
       <c r="V47" s="14"/>
@@ -20793,34 +21052,40 @@
         <v>97</v>
       </c>
       <c r="B48" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="C48" s="14">
+        <v>0</v>
+      </c>
+      <c r="D48" s="52" t="s">
+        <v>579</v>
+      </c>
+      <c r="E48" s="56" t="s">
+        <v>580</v>
+      </c>
+      <c r="F48" s="51">
+        <v>2017</v>
+      </c>
+      <c r="G48" s="35" t="s">
+        <v>581</v>
+      </c>
+      <c r="H48" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>582</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="K48" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="L48" s="41">
+        <v>4</v>
+      </c>
+      <c r="M48" s="16" t="s">
         <v>584</v>
-      </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="53" t="s">
-        <v>585</v>
-      </c>
-      <c r="E48" s="57" t="s">
-        <v>586</v>
-      </c>
-      <c r="F48" s="52">
-        <v>2017</v>
-      </c>
-      <c r="G48" s="35" t="s">
-        <v>587</v>
-      </c>
-      <c r="H48" s="41"/>
-      <c r="I48" s="16" t="s">
-        <v>588</v>
-      </c>
-      <c r="J48" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="K48" s="16" t="s">
-        <v>589</v>
-      </c>
-      <c r="L48" s="41"/>
-      <c r="M48" s="16" t="s">
-        <v>590</v>
       </c>
       <c r="N48" s="14"/>
       <c r="O48" s="14"/>
@@ -20829,7 +21094,7 @@
       <c r="R48" s="14"/>
       <c r="S48" s="14"/>
       <c r="T48" s="16" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="U48" s="41"/>
       <c r="V48" s="14"/>
@@ -20845,45 +21110,51 @@
         <v>40</v>
       </c>
       <c r="B49" s="10" t="s">
+        <v>621</v>
+      </c>
+      <c r="C49" s="14">
+        <v>3</v>
+      </c>
+      <c r="D49" s="52" t="s">
+        <v>586</v>
+      </c>
+      <c r="E49" s="56" t="s">
+        <v>587</v>
+      </c>
+      <c r="F49" s="51">
+        <v>2019</v>
+      </c>
+      <c r="G49" s="35" t="s">
+        <v>588</v>
+      </c>
+      <c r="H49" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="K49" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="L49" s="41">
+        <v>18</v>
+      </c>
+      <c r="M49" s="16" t="s">
         <v>592</v>
-      </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="53" t="s">
-        <v>592</v>
-      </c>
-      <c r="E49" s="57" t="s">
-        <v>593</v>
-      </c>
-      <c r="F49" s="52">
-        <v>2019</v>
-      </c>
-      <c r="G49" s="35" t="s">
-        <v>594</v>
-      </c>
-      <c r="H49" s="41"/>
-      <c r="I49" s="16" t="s">
-        <v>595</v>
-      </c>
-      <c r="J49" s="12" t="s">
-        <v>596</v>
-      </c>
-      <c r="K49" s="16" t="s">
-        <v>597</v>
-      </c>
-      <c r="L49" s="41"/>
-      <c r="M49" s="16" t="s">
-        <v>598</v>
       </c>
       <c r="N49" s="14"/>
       <c r="O49" s="12" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="P49" s="14"/>
       <c r="Q49" s="14"/>
       <c r="R49" s="14"/>
       <c r="S49" s="14"/>
       <c r="T49" s="16" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="U49" s="41"/>
       <c r="V49" s="14"/>

</xml_diff>

<commit_message>
It was removed a paper duplicated
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form.xlsx
+++ b/dataset/Extraction_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="15260"/>
+    <workbookView xWindow="40" yWindow="240" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Folha 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="634">
   <si>
     <t>Citation</t>
   </si>
@@ -4961,12 +4961,6 @@
     </r>
   </si>
   <si>
-    <t>Tommasel, A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Applying Social Network Analysis Techniques to Architectural Smell Prediction  </t>
-  </si>
-  <si>
     <t>Li et al. 2015</t>
   </si>
   <si>
@@ -15997,18 +15991,7 @@
     <t>Book series</t>
   </si>
   <si>
-    <t>Measurement,Social networking (online),Computer architecture,Software architecture,Software systems,Software design</t>
-  </si>
-  <si>
-    <t>Identify architectural smells using SNA (Social Network Analysis) via graph based approuch to make predictions about software design dependencies, evolution and properties of the system.</t>
-  </si>
-  <si>
     <t>Not available</t>
-  </si>
-  <si>
-    <t>The ongoing research has primary focused on the definition of the dependency graph and the evaluation of the depend- ency predictor. The definition of the dependency graph was complemented with a statistical analysis of software versions and the evolution of SNA metrics (tackling RQ1). In this line, it was analysed how past decisions reflected in the software structure affect the future occurrence of dependencies, and smells thereof (tackling RQ3). In addition, it was analysed the descriptive power of both topological and content-based fea- tures for defining the similarity of components (tackling RQ2). The descriptive power of software-related metrics remains to be evaluated. Regarding smell prediction, evaluations focused on defining preliminary filtering strategies for cycles and hubs (tackling RQ4).
-At present, the research is oriented to perform a systematic study with more systems (and versions) to corroborate the initial findings reported in [9, 10]. Moreover, considering the errors in which learned models could incur, additional studies are being performed to introduce mechanisms of reinforcement learning to feed the predictions with new information obtained from the environment (or from the architect), as a means to establish the confidence of predictions and reducing the probability of false positives.
-Once the prediction technique is fully evaluated, it will be incorporated into a tool to evaluate the capabilities of the approach in a study with subjects in the context of real software projects. Finally, it is expected to include other types of architectural smells [15] in the work.</t>
   </si>
   <si>
     <t>2</t>
@@ -16329,7 +16312,7 @@
       <name val="Times Roman"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -16339,12 +16322,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -16483,7 +16460,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -16546,11 +16523,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
@@ -17799,11 +17771,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB49"/>
+  <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -17835,7 +17807,7 @@
   <sheetData>
     <row r="1" spans="1:28" ht="28" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -17844,52 +17816,52 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>597</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>598</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>600</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>603</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>605</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>4</v>
@@ -17898,25 +17870,25 @@
         <v>5</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="W1" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>615</v>
-      </c>
       <c r="Y1" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>607</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="355" customHeight="1">
@@ -17930,7 +17902,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
@@ -18234,7 +18206,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C6" s="11">
         <v>4</v>
@@ -18464,7 +18436,7 @@
         <v>129</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>130</v>
@@ -18676,7 +18648,7 @@
         <v>172</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>173</v>
@@ -18710,7 +18682,7 @@
       </c>
       <c r="S12" s="14"/>
       <c r="T12" s="14" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="U12" s="14"/>
       <c r="V12" s="12" t="s">
@@ -18818,7 +18790,7 @@
         <v>200</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>201</v>
@@ -18863,56 +18835,70 @@
       <c r="AA14" s="14"/>
       <c r="AB14" s="14"/>
     </row>
-    <row r="15" spans="1:28" ht="238" customHeight="1">
+    <row r="15" spans="1:28" ht="409.5" customHeight="1">
       <c r="A15" s="9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>635</v>
-      </c>
-      <c r="D15" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="C15" s="22">
+        <v>36</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="F15" s="23">
-        <v>2019</v>
+      <c r="E15" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="F15" s="9">
+        <v>2015</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>314</v>
+        <v>213</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="J15" s="14" t="s">
+      <c r="I15" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L15" s="13">
+        <v>10</v>
+      </c>
+      <c r="M15" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="K15" s="14" t="s">
-        <v>631</v>
-      </c>
-      <c r="L15" s="14">
-        <v>8</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>632</v>
-      </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14" t="s">
-        <v>634</v>
-      </c>
-      <c r="U15" s="14"/>
+      <c r="N15" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="R15" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="S15" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="T15" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="U15" s="12" t="s">
+        <v>224</v>
+      </c>
       <c r="V15" s="14"/>
       <c r="W15" s="14"/>
       <c r="X15" s="14"/>
@@ -18921,69 +18907,69 @@
       <c r="AA15" s="14"/>
       <c r="AB15" s="14"/>
     </row>
-    <row r="16" spans="1:28" ht="409.5" customHeight="1">
+    <row r="16" spans="1:28" ht="320.25" customHeight="1">
       <c r="A16" s="9">
-        <v>21</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="C16" s="25">
-        <v>36</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>213</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>214</v>
+        <v>22</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="9">
+        <v>75</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>227</v>
       </c>
       <c r="F16" s="9">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="H16" s="14" t="s">
         <v>44</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="L16" s="13">
-        <v>10</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>219</v>
+        <v>230</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="L16" s="14">
+        <v>8</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>232</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="R16" s="12" t="s">
-        <v>138</v>
+        <v>237</v>
       </c>
       <c r="S16" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="T16" s="10" t="s">
-        <v>225</v>
+        <v>238</v>
+      </c>
+      <c r="T16" s="12" t="s">
+        <v>239</v>
       </c>
       <c r="U16" s="12" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="V16" s="14"/>
       <c r="W16" s="14"/>
@@ -18993,69 +18979,69 @@
       <c r="AA16" s="14"/>
       <c r="AB16" s="14"/>
     </row>
-    <row r="17" spans="1:28" ht="320.25" customHeight="1">
+    <row r="17" spans="1:28" ht="409.5" customHeight="1">
       <c r="A17" s="9">
-        <v>22</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="C17" s="9">
-        <v>75</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>228</v>
+        <v>27</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="11">
+        <v>9</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="F17" s="9">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>44</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>232</v>
+        <v>131</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="L17" s="14">
         <v>8</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="R17" s="12" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="S17" s="12" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="U17" s="12" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="V17" s="14"/>
       <c r="W17" s="14"/>
@@ -19067,67 +19053,67 @@
     </row>
     <row r="18" spans="1:28" ht="409.5" customHeight="1">
       <c r="A18" s="9">
-        <v>27</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" s="11">
-        <v>9</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>243</v>
+        <v>30</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C18" s="9">
+        <v>13</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>256</v>
       </c>
       <c r="F18" s="9">
-        <v>2016</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>244</v>
+        <v>2018</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>257</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>44</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>245</v>
+        <v>258</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>246</v>
+        <v>215</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>629</v>
       </c>
       <c r="L18" s="14">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>250</v>
+        <v>261</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>262</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="R18" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="S18" s="12" t="s">
-        <v>253</v>
+        <v>264</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>265</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="U18" s="12" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="V18" s="14"/>
       <c r="W18" s="14"/>
@@ -19137,69 +19123,69 @@
       <c r="AA18" s="14"/>
       <c r="AB18" s="14"/>
     </row>
-    <row r="19" spans="1:28" ht="409.5" customHeight="1">
+    <row r="19" spans="1:28" ht="372.25" customHeight="1">
       <c r="A19" s="9">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="C19" s="9">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="F19" s="9">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>44</v>
+        <v>626</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>217</v>
+        <v>273</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="L19" s="14">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="P19" s="10" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="Q19" s="12" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="R19" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="S19" s="10" t="s">
-        <v>267</v>
+        <v>279</v>
+      </c>
+      <c r="S19" s="12" t="s">
+        <v>280</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="U19" s="12" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="V19" s="14"/>
       <c r="W19" s="14"/>
@@ -19209,69 +19195,69 @@
       <c r="AA19" s="14"/>
       <c r="AB19" s="14"/>
     </row>
-    <row r="20" spans="1:28" ht="372.25" customHeight="1">
+    <row r="20" spans="1:28" ht="409.5" customHeight="1">
       <c r="A20" s="9">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="C20" s="9">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="F20" s="9">
-        <v>2016</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>273</v>
+        <v>2015</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>286</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>628</v>
+        <v>44</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="L20" s="14">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="O20" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="P20" s="10" t="s">
-        <v>279</v>
+        <v>290</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>292</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="S20" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="T20" s="12" t="s">
-        <v>283</v>
+        <v>294</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="T20" s="10" t="s">
+        <v>296</v>
       </c>
       <c r="U20" s="12" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="V20" s="14"/>
       <c r="W20" s="14"/>
@@ -19281,70 +19267,64 @@
       <c r="AA20" s="14"/>
       <c r="AB20" s="14"/>
     </row>
-    <row r="21" spans="1:28" ht="409.5" customHeight="1">
-      <c r="A21" s="9">
-        <v>48</v>
+    <row r="21" spans="1:28" ht="333.25" customHeight="1">
+      <c r="A21" s="23">
+        <v>47</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="C21" s="9">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>287</v>
+        <v>127</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>299</v>
       </c>
       <c r="F21" s="9">
         <v>2015</v>
       </c>
-      <c r="G21" s="18" t="s">
-        <v>288</v>
+      <c r="G21" s="10" t="s">
+        <v>300</v>
       </c>
       <c r="H21" s="14" t="s">
         <v>44</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="K21" s="14" t="s">
-        <v>638</v>
+        <v>46</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>302</v>
       </c>
       <c r="L21" s="14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M21" s="12" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="O21" s="10" t="s">
-        <v>293</v>
+        <v>304</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>305</v>
       </c>
       <c r="P21" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q21" s="12" t="s">
-        <v>295</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="Q21" s="14"/>
       <c r="R21" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="S21" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="T21" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="U21" s="12" t="s">
-        <v>299</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="S21" s="14"/>
+      <c r="T21" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="U21" s="14"/>
       <c r="V21" s="14"/>
       <c r="W21" s="14"/>
       <c r="X21" s="14"/>
@@ -19353,64 +19333,62 @@
       <c r="AA21" s="14"/>
       <c r="AB21" s="14"/>
     </row>
-    <row r="22" spans="1:28" ht="333.25" customHeight="1">
-      <c r="A22" s="26">
-        <v>47</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="C22" s="9">
-        <v>21</v>
+    <row r="22" spans="1:28" ht="409.5" customHeight="1">
+      <c r="A22" s="9">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>630</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>127</v>
+        <v>310</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="F22" s="9">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="H22" s="14" t="s">
         <v>44</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>46</v>
+        <v>215</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="L22" s="14">
         <v>8</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>306</v>
-      </c>
-      <c r="O22" s="12" t="s">
-        <v>307</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
       <c r="P22" s="12" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="Q22" s="14"/>
       <c r="R22" s="12" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="S22" s="14"/>
-      <c r="T22" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="U22" s="14"/>
+      <c r="T22" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="U22" s="12" t="s">
+        <v>319</v>
+      </c>
       <c r="V22" s="14"/>
       <c r="W22" s="14"/>
       <c r="X22" s="14"/>
@@ -19421,59 +19399,61 @@
     </row>
     <row r="23" spans="1:28" ht="409.5" customHeight="1">
       <c r="A23" s="9">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>61</v>
+        <v>320</v>
+      </c>
+      <c r="C23" s="9">
+        <v>137</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="F23" s="9">
-        <v>2019</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="H23" s="14" t="s">
+        <v>2012</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="H23" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="12" t="s">
-        <v>315</v>
+      <c r="I23" s="18" t="s">
+        <v>324</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="L23" s="14">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
+      <c r="O23" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="P23" s="12" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="Q23" s="14"/>
-      <c r="R23" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="S23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="12" t="s">
+        <v>329</v>
+      </c>
       <c r="T23" s="10" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="U23" s="12" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="V23" s="14"/>
       <c r="W23" s="14"/>
@@ -19483,63 +19463,69 @@
       <c r="AA23" s="14"/>
       <c r="AB23" s="14"/>
     </row>
-    <row r="24" spans="1:28" ht="409.5" customHeight="1">
+    <row r="24" spans="1:28" ht="345.25" customHeight="1">
       <c r="A24" s="9">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="C24" s="9">
-        <v>137</v>
+        <v>332</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>323</v>
+        <v>269</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="F24" s="9">
-        <v>2012</v>
+        <v>2019</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>325</v>
-      </c>
-      <c r="H24" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="H24" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="18" t="s">
-        <v>326</v>
+      <c r="I24" s="10" t="s">
+        <v>335</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>327</v>
+        <v>174</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>336</v>
       </c>
       <c r="L24" s="14">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="N24" s="14"/>
+        <v>337</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>338</v>
+      </c>
       <c r="O24" s="12" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
+        <v>340</v>
+      </c>
+      <c r="Q24" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="R24" s="12" t="s">
+        <v>250</v>
+      </c>
       <c r="S24" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="T24" s="10" t="s">
-        <v>332</v>
+        <v>342</v>
+      </c>
+      <c r="T24" s="16" t="s">
+        <v>343</v>
       </c>
       <c r="U24" s="12" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="V24" s="14"/>
       <c r="W24" s="14"/>
@@ -19549,69 +19535,63 @@
       <c r="AA24" s="14"/>
       <c r="AB24" s="14"/>
     </row>
-    <row r="25" spans="1:28" ht="345.25" customHeight="1">
+    <row r="25" spans="1:28" ht="409.5" customHeight="1">
       <c r="A25" s="9">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="C25" s="9">
+        <v>5</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>335</v>
+        <v>345</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>346</v>
       </c>
       <c r="F25" s="9">
-        <v>2019</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>336</v>
-      </c>
-      <c r="H25" s="13" t="s">
+        <v>2018</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="H25" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>337</v>
+      <c r="I25" s="26" t="s">
+        <v>348</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="L25" s="14">
-        <v>2</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>339</v>
+        <v>131</v>
+      </c>
+      <c r="K25" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="L25" s="13">
+        <v>4</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>350</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="P25" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q25" s="12" t="s">
-        <v>343</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
       <c r="R25" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="S25" s="12" t="s">
-        <v>344</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="S25" s="14"/>
       <c r="T25" s="16" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="U25" s="12" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="V25" s="14"/>
       <c r="W25" s="14"/>
@@ -19623,61 +19603,67 @@
     </row>
     <row r="26" spans="1:28" ht="409.5" customHeight="1">
       <c r="A26" s="9">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>60</v>
+        <v>356</v>
       </c>
       <c r="C26" s="9">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>348</v>
+        <v>357</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>358</v>
       </c>
       <c r="F26" s="9">
-        <v>2018</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="H26" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="29" t="s">
-        <v>350</v>
+        <v>2015</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>626</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>360</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K26" s="30" t="s">
-        <v>351</v>
+        <v>174</v>
+      </c>
+      <c r="K26" s="27" t="s">
+        <v>361</v>
       </c>
       <c r="L26" s="13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="O26" s="12" t="s">
-        <v>354</v>
-      </c>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
+        <v>364</v>
+      </c>
+      <c r="P26" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q26" s="12" t="s">
+        <v>366</v>
+      </c>
       <c r="R26" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="S26" s="14"/>
+        <v>367</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>365</v>
+      </c>
       <c r="T26" s="16" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="U26" s="12" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="V26" s="14"/>
       <c r="W26" s="14"/>
@@ -19689,68 +19675,58 @@
     </row>
     <row r="27" spans="1:28" ht="409.5" customHeight="1">
       <c r="A27" s="9">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>358</v>
+        <v>197</v>
       </c>
       <c r="C27" s="9">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>359</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>360</v>
+        <v>198</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>370</v>
       </c>
       <c r="F27" s="9">
-        <v>2015</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>361</v>
-      </c>
-      <c r="H27" s="28" t="s">
-        <v>628</v>
-      </c>
-      <c r="I27" s="29" t="s">
-        <v>362</v>
+        <v>2016</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>626</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>372</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="K27" s="30" t="s">
-        <v>363</v>
+      <c r="K27" s="10" t="s">
+        <v>373</v>
       </c>
       <c r="L27" s="13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>366</v>
-      </c>
-      <c r="P27" s="12" t="s">
-        <v>367</v>
-      </c>
-      <c r="Q27" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="R27" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="S27" s="12" t="s">
-        <v>367</v>
-      </c>
-      <c r="T27" s="16" t="s">
-        <v>370</v>
-      </c>
-      <c r="U27" s="12" t="s">
-        <v>371</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="U27" s="14"/>
       <c r="V27" s="14"/>
       <c r="W27" s="14"/>
       <c r="X27" s="14"/>
@@ -19759,60 +19735,62 @@
       <c r="AA27" s="14"/>
       <c r="AB27" s="14"/>
     </row>
-    <row r="28" spans="1:28" ht="409.5" customHeight="1">
+    <row r="28" spans="1:28" ht="358.25" customHeight="1">
       <c r="A28" s="9">
-        <v>44</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="C28" s="9">
-        <v>23</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="F28" s="9">
+        <v>43</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>617</v>
+      </c>
+      <c r="C28" s="14">
+        <v>35</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>616</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="F28" s="29">
         <v>2016</v>
       </c>
-      <c r="G28" s="10" t="s">
-        <v>373</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>628</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>374</v>
+      <c r="G28" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>380</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>375</v>
+        <v>381</v>
+      </c>
+      <c r="K28" s="27" t="s">
+        <v>382</v>
       </c>
       <c r="L28" s="13">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="O28" s="12" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="P28" s="14"/>
       <c r="Q28" s="14"/>
       <c r="R28" s="14"/>
       <c r="S28" s="14"/>
-      <c r="T28" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="U28" s="14"/>
+      <c r="T28" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="U28" s="12" t="s">
+        <v>387</v>
+      </c>
       <c r="V28" s="14"/>
       <c r="W28" s="14"/>
       <c r="X28" s="14"/>
@@ -19821,61 +19799,65 @@
       <c r="AA28" s="14"/>
       <c r="AB28" s="14"/>
     </row>
-    <row r="29" spans="1:28" ht="358.25" customHeight="1">
+    <row r="29" spans="1:28" ht="333.25" customHeight="1">
       <c r="A29" s="9">
-        <v>43</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>619</v>
-      </c>
-      <c r="C29" s="14">
-        <v>35</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>618</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>380</v>
-      </c>
-      <c r="F29" s="32">
-        <v>2016</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="H29" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>382</v>
+        <v>51</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="C29" s="9">
+        <v>3</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="F29" s="9">
+        <v>2019</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>392</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>383</v>
-      </c>
-      <c r="K29" s="30" t="s">
-        <v>384</v>
+        <v>393</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>394</v>
       </c>
       <c r="L29" s="13">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="N29" s="12" t="s">
-        <v>386</v>
-      </c>
+        <v>395</v>
+      </c>
+      <c r="N29" s="14"/>
       <c r="O29" s="12" t="s">
-        <v>387</v>
-      </c>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
+        <v>396</v>
+      </c>
+      <c r="P29" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q29" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="R29" s="12" t="s">
+        <v>399</v>
+      </c>
       <c r="S29" s="14"/>
-      <c r="T29" s="16" t="s">
-        <v>388</v>
+      <c r="T29" s="10" t="s">
+        <v>400</v>
       </c>
       <c r="U29" s="12" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="V29" s="14"/>
       <c r="W29" s="14"/>
@@ -19885,65 +19867,65 @@
       <c r="AA29" s="14"/>
       <c r="AB29" s="14"/>
     </row>
-    <row r="30" spans="1:28" ht="333.25" customHeight="1">
+    <row r="30" spans="1:28" ht="409.5" customHeight="1">
       <c r="A30" s="9">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="C30" s="9">
         <v>3</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="F30" s="9">
         <v>2019</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="H30" s="13" t="s">
         <v>44</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>395</v>
+        <v>215</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="L30" s="13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M30" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="O30" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="P30" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="N30" s="14"/>
-      <c r="O30" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="P30" s="12" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q30" s="12" t="s">
-        <v>400</v>
-      </c>
+      <c r="Q30" s="14"/>
       <c r="R30" s="12" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="S30" s="14"/>
       <c r="T30" s="10" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="U30" s="12" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="V30" s="14"/>
       <c r="W30" s="14"/>
@@ -19955,63 +19937,61 @@
     </row>
     <row r="31" spans="1:28" ht="409.5" customHeight="1">
       <c r="A31" s="9">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="C31" s="9">
-        <v>3</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>405</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>406</v>
+        <v>4</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>415</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>416</v>
       </c>
       <c r="F31" s="9">
         <v>2019</v>
       </c>
-      <c r="G31" s="10" t="s">
-        <v>407</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>408</v>
+      <c r="G31" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="H31" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="34" t="s">
+        <v>418</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>217</v>
+        <v>131</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="L31" s="13">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="O31" s="12" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="P31" s="12" t="s">
-        <v>399</v>
+        <v>423</v>
       </c>
       <c r="Q31" s="14"/>
-      <c r="R31" s="12" t="s">
-        <v>413</v>
-      </c>
+      <c r="R31" s="14"/>
       <c r="S31" s="14"/>
       <c r="T31" s="10" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="U31" s="12" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="V31" s="14"/>
       <c r="W31" s="14"/>
@@ -20023,61 +20003,63 @@
     </row>
     <row r="32" spans="1:28" ht="409.5" customHeight="1">
       <c r="A32" s="9">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="C32" s="9">
-        <v>4</v>
-      </c>
-      <c r="D32" s="33" t="s">
-        <v>417</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>418</v>
+        <v>8</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>427</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>428</v>
       </c>
       <c r="F32" s="9">
-        <v>2019</v>
-      </c>
-      <c r="G32" s="35" t="s">
-        <v>419</v>
-      </c>
-      <c r="H32" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="I32" s="37" t="s">
-        <v>420</v>
+        <v>2018</v>
+      </c>
+      <c r="G32" s="27" t="s">
+        <v>429</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="I32" s="34" t="s">
+        <v>430</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="L32" s="13">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>423</v>
-      </c>
-      <c r="O32" s="12" t="s">
-        <v>424</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="O32" s="14"/>
       <c r="P32" s="12" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
       <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
+      <c r="R32" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="S32" s="12" t="s">
+        <v>435</v>
+      </c>
       <c r="T32" s="10" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="U32" s="12" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="V32" s="14"/>
       <c r="W32" s="14"/>
@@ -20089,63 +20071,65 @@
     </row>
     <row r="33" spans="1:28" ht="409.5" customHeight="1">
       <c r="A33" s="9">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>428</v>
+        <v>618</v>
       </c>
       <c r="C33" s="9">
-        <v>8</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>429</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>430</v>
+        <v>21</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>439</v>
       </c>
       <c r="F33" s="9">
-        <v>2018</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>431</v>
-      </c>
-      <c r="H33" s="36" t="s">
+        <v>2017</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="H33" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="I33" s="37" t="s">
-        <v>432</v>
+      <c r="I33" s="34" t="s">
+        <v>441</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="K33" s="10" t="s">
-        <v>433</v>
+        <v>393</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>442</v>
       </c>
       <c r="L33" s="13">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="M33" s="10" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>435</v>
-      </c>
-      <c r="O33" s="14"/>
+        <v>444</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>445</v>
+      </c>
       <c r="P33" s="12" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="Q33" s="14"/>
       <c r="R33" s="12" t="s">
-        <v>252</v>
+        <v>447</v>
       </c>
       <c r="S33" s="12" t="s">
-        <v>437</v>
+        <v>448</v>
       </c>
       <c r="T33" s="10" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
       <c r="U33" s="12" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="V33" s="14"/>
       <c r="W33" s="14"/>
@@ -20157,65 +20141,59 @@
     </row>
     <row r="34" spans="1:28" ht="409.5" customHeight="1">
       <c r="A34" s="9">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>620</v>
+        <v>451</v>
       </c>
       <c r="C34" s="9">
-        <v>21</v>
-      </c>
-      <c r="D34" s="33" t="s">
-        <v>440</v>
-      </c>
-      <c r="E34" s="38" t="s">
-        <v>441</v>
+        <v>28</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>452</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>453</v>
       </c>
       <c r="F34" s="9">
-        <v>2017</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>442</v>
-      </c>
-      <c r="H34" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="I34" s="37" t="s">
-        <v>443</v>
+        <v>2016</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>454</v>
+      </c>
+      <c r="H34" s="33" t="s">
+        <v>626</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>455</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>395</v>
+        <v>174</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="L34" s="13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M34" s="10" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="O34" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="P34" s="12" t="s">
-        <v>448</v>
-      </c>
+        <v>459</v>
+      </c>
+      <c r="P34" s="14"/>
       <c r="Q34" s="14"/>
-      <c r="R34" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="S34" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="T34" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="U34" s="12" t="s">
-        <v>452</v>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="16" t="s">
+        <v>460</v>
+      </c>
+      <c r="U34" s="16" t="s">
+        <v>461</v>
       </c>
       <c r="V34" s="14"/>
       <c r="W34" s="14"/>
@@ -20227,59 +20205,59 @@
     </row>
     <row r="35" spans="1:28" ht="409.5" customHeight="1">
       <c r="A35" s="9">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="C35" s="9">
-        <v>28</v>
-      </c>
-      <c r="D35" s="33" t="s">
-        <v>454</v>
-      </c>
-      <c r="E35" s="34" t="s">
-        <v>455</v>
+        <v>12</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>463</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>464</v>
       </c>
       <c r="F35" s="9">
         <v>2016</v>
       </c>
-      <c r="G35" s="39" t="s">
-        <v>456</v>
-      </c>
-      <c r="H35" s="36" t="s">
-        <v>628</v>
-      </c>
-      <c r="I35" s="37" t="s">
-        <v>457</v>
+      <c r="G35" s="36" t="s">
+        <v>465</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="I35" s="34" t="s">
+        <v>466</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>174</v>
+        <v>288</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
       <c r="L35" s="13">
         <v>8</v>
       </c>
       <c r="M35" s="10" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="O35" s="12" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="P35" s="14"/>
       <c r="Q35" s="14"/>
       <c r="R35" s="14"/>
       <c r="S35" s="14"/>
       <c r="T35" s="16" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="U35" s="16" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="V35" s="14"/>
       <c r="W35" s="14"/>
@@ -20291,60 +20269,66 @@
     </row>
     <row r="36" spans="1:28" ht="409.5" customHeight="1">
       <c r="A36" s="9">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="C36" s="9">
-        <v>12</v>
-      </c>
-      <c r="D36" s="33" t="s">
-        <v>465</v>
-      </c>
-      <c r="E36" s="40" t="s">
-        <v>466</v>
+        <v>0</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>474</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>475</v>
       </c>
       <c r="F36" s="9">
-        <v>2016</v>
-      </c>
-      <c r="G36" s="39" t="s">
-        <v>467</v>
-      </c>
-      <c r="H36" s="36" t="s">
+        <v>2017</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>476</v>
+      </c>
+      <c r="H36" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="I36" s="37" t="s">
-        <v>468</v>
+      <c r="I36" s="34" t="s">
+        <v>627</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>290</v>
+        <v>477</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>469</v>
-      </c>
-      <c r="L36" s="13">
-        <v>8</v>
-      </c>
-      <c r="M36" s="10" t="s">
-        <v>470</v>
+        <v>478</v>
+      </c>
+      <c r="L36" s="38">
+        <v>10</v>
+      </c>
+      <c r="M36" s="16" t="s">
+        <v>479</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="O36" s="12" t="s">
-        <v>472</v>
-      </c>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
+        <v>481</v>
+      </c>
+      <c r="P36" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q36" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="R36" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="S36" s="12" t="s">
+        <v>482</v>
+      </c>
       <c r="T36" s="16" t="s">
-        <v>473</v>
-      </c>
-      <c r="U36" s="16" t="s">
-        <v>474</v>
-      </c>
+        <v>484</v>
+      </c>
+      <c r="U36" s="38"/>
       <c r="V36" s="14"/>
       <c r="W36" s="14"/>
       <c r="X36" s="14"/>
@@ -20355,66 +20339,58 @@
     </row>
     <row r="37" spans="1:28" ht="409.5" customHeight="1">
       <c r="A37" s="9">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C37" s="9">
-        <v>0</v>
-      </c>
-      <c r="D37" s="33" t="s">
-        <v>476</v>
-      </c>
-      <c r="E37" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>621</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="F37" s="9">
+        <v>2015</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>487</v>
+      </c>
+      <c r="H37" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" s="34" t="s">
+        <v>488</v>
+      </c>
+      <c r="J37" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="F37" s="9">
-        <v>2017</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>478</v>
-      </c>
-      <c r="H37" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="I37" s="37" t="s">
-        <v>629</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>479</v>
-      </c>
-      <c r="K37" s="16" t="s">
-        <v>480</v>
-      </c>
-      <c r="L37" s="41">
-        <v>10</v>
+      <c r="K37" s="39" t="s">
+        <v>489</v>
+      </c>
+      <c r="L37" s="38">
+        <v>17</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>482</v>
+        <v>491</v>
       </c>
       <c r="O37" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="P37" s="12" t="s">
-        <v>484</v>
-      </c>
-      <c r="Q37" s="12" t="s">
-        <v>485</v>
-      </c>
-      <c r="R37" s="12" t="s">
-        <v>484</v>
-      </c>
-      <c r="S37" s="12" t="s">
-        <v>484</v>
-      </c>
+        <v>492</v>
+      </c>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
       <c r="T37" s="16" t="s">
-        <v>486</v>
-      </c>
-      <c r="U37" s="41"/>
+        <v>493</v>
+      </c>
+      <c r="U37" s="38"/>
       <c r="V37" s="14"/>
       <c r="W37" s="14"/>
       <c r="X37" s="14"/>
@@ -20425,58 +20401,56 @@
     </row>
     <row r="38" spans="1:28" ht="409.5" customHeight="1">
       <c r="A38" s="9">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="C38" s="9">
-        <v>65</v>
-      </c>
-      <c r="D38" s="33" t="s">
-        <v>623</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>488</v>
+        <v>15</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>495</v>
+      </c>
+      <c r="E38" s="40" t="s">
+        <v>496</v>
       </c>
       <c r="F38" s="9">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>489</v>
-      </c>
-      <c r="H38" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="I38" s="37" t="s">
-        <v>490</v>
+        <v>497</v>
+      </c>
+      <c r="H38" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="I38" s="41" t="s">
+        <v>498</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>479</v>
-      </c>
-      <c r="K38" s="42" t="s">
-        <v>491</v>
-      </c>
-      <c r="L38" s="41">
-        <v>17</v>
+        <v>131</v>
+      </c>
+      <c r="K38" s="39" t="s">
+        <v>499</v>
+      </c>
+      <c r="L38" s="38">
+        <v>27</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>493</v>
-      </c>
-      <c r="O38" s="12" t="s">
-        <v>494</v>
-      </c>
+        <v>501</v>
+      </c>
+      <c r="O38" s="14"/>
       <c r="P38" s="14"/>
       <c r="Q38" s="14"/>
       <c r="R38" s="14"/>
       <c r="S38" s="14"/>
       <c r="T38" s="16" t="s">
-        <v>495</v>
-      </c>
-      <c r="U38" s="41"/>
+        <v>502</v>
+      </c>
+      <c r="U38" s="38"/>
       <c r="V38" s="14"/>
       <c r="W38" s="14"/>
       <c r="X38" s="14"/>
@@ -20487,46 +20461,46 @@
     </row>
     <row r="39" spans="1:28" ht="409.5" customHeight="1">
       <c r="A39" s="9">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="C39" s="9">
-        <v>15</v>
-      </c>
-      <c r="D39" s="33" t="s">
-        <v>497</v>
-      </c>
-      <c r="E39" s="43" t="s">
-        <v>498</v>
+        <v>9</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>504</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>505</v>
       </c>
       <c r="F39" s="9">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="H39" s="57" t="s">
+        <v>506</v>
+      </c>
+      <c r="H39" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="I39" s="44" t="s">
-        <v>500</v>
+      <c r="I39" s="26" t="s">
+        <v>507</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="K39" s="42" t="s">
-        <v>501</v>
-      </c>
-      <c r="L39" s="41">
-        <v>27</v>
+        <v>393</v>
+      </c>
+      <c r="K39" s="39" t="s">
+        <v>508</v>
+      </c>
+      <c r="L39" s="38">
+        <v>11</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="O39" s="14"/>
       <c r="P39" s="14"/>
@@ -20534,9 +20508,9 @@
       <c r="R39" s="14"/>
       <c r="S39" s="14"/>
       <c r="T39" s="16" t="s">
-        <v>504</v>
-      </c>
-      <c r="U39" s="41"/>
+        <v>511</v>
+      </c>
+      <c r="U39" s="38"/>
       <c r="V39" s="14"/>
       <c r="W39" s="14"/>
       <c r="X39" s="14"/>
@@ -20545,48 +20519,48 @@
       <c r="AA39" s="14"/>
       <c r="AB39" s="14"/>
     </row>
-    <row r="40" spans="1:28" ht="409.5" customHeight="1">
+    <row r="40" spans="1:28" ht="318.25" customHeight="1">
       <c r="A40" s="9">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>505</v>
-      </c>
-      <c r="C40" s="9">
-        <v>9</v>
-      </c>
-      <c r="D40" s="33" t="s">
-        <v>506</v>
-      </c>
-      <c r="E40" s="31" t="s">
-        <v>507</v>
+        <v>512</v>
+      </c>
+      <c r="C40" s="14">
+        <v>12</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>622</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>513</v>
       </c>
       <c r="F40" s="9">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>508</v>
-      </c>
-      <c r="H40" s="28" t="s">
+        <v>514</v>
+      </c>
+      <c r="H40" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="I40" s="29" t="s">
-        <v>509</v>
-      </c>
-      <c r="J40" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="K40" s="42" t="s">
-        <v>510</v>
-      </c>
-      <c r="L40" s="41">
-        <v>11</v>
+      <c r="I40" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="K40" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="L40" s="38">
+        <v>5</v>
       </c>
       <c r="M40" s="16" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="O40" s="14"/>
       <c r="P40" s="14"/>
@@ -20594,9 +20568,9 @@
       <c r="R40" s="14"/>
       <c r="S40" s="14"/>
       <c r="T40" s="16" t="s">
-        <v>513</v>
-      </c>
-      <c r="U40" s="41"/>
+        <v>519</v>
+      </c>
+      <c r="U40" s="38"/>
       <c r="V40" s="14"/>
       <c r="W40" s="14"/>
       <c r="X40" s="14"/>
@@ -20605,58 +20579,60 @@
       <c r="AA40" s="14"/>
       <c r="AB40" s="14"/>
     </row>
-    <row r="41" spans="1:28" ht="318.25" customHeight="1">
+    <row r="41" spans="1:28" ht="404.25" customHeight="1">
       <c r="A41" s="9">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>514</v>
+        <v>615</v>
       </c>
       <c r="C41" s="14">
-        <v>12</v>
-      </c>
-      <c r="D41" s="45" t="s">
-        <v>624</v>
-      </c>
-      <c r="E41" s="31" t="s">
-        <v>515</v>
+        <v>105</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>520</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>521</v>
       </c>
       <c r="F41" s="9">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>516</v>
-      </c>
-      <c r="H41" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="I41" s="29" t="s">
-        <v>517</v>
-      </c>
-      <c r="J41" s="14" t="s">
-        <v>131</v>
+        <v>522</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>174</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>518</v>
-      </c>
-      <c r="L41" s="41">
-        <v>5</v>
+        <v>524</v>
+      </c>
+      <c r="L41" s="38">
+        <v>9</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>520</v>
-      </c>
-      <c r="O41" s="14"/>
+        <v>526</v>
+      </c>
+      <c r="O41" s="12" t="s">
+        <v>481</v>
+      </c>
       <c r="P41" s="14"/>
       <c r="Q41" s="14"/>
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
       <c r="T41" s="16" t="s">
-        <v>521</v>
-      </c>
-      <c r="U41" s="41"/>
+        <v>527</v>
+      </c>
+      <c r="U41" s="38"/>
       <c r="V41" s="14"/>
       <c r="W41" s="14"/>
       <c r="X41" s="14"/>
@@ -20665,60 +20641,62 @@
       <c r="AA41" s="14"/>
       <c r="AB41" s="14"/>
     </row>
-    <row r="42" spans="1:28" ht="404.25" customHeight="1">
+    <row r="42" spans="1:28" ht="398.75" customHeight="1">
       <c r="A42" s="9">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C42" s="14">
-        <v>105</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>522</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>523</v>
+        <v>103</v>
+      </c>
+      <c r="D42" s="43" t="s">
+        <v>520</v>
+      </c>
+      <c r="E42" s="44" t="s">
+        <v>528</v>
       </c>
       <c r="F42" s="9">
         <v>2012</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>524</v>
-      </c>
-      <c r="H42" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="I42" s="29" t="s">
-        <v>525</v>
+        <v>529</v>
+      </c>
+      <c r="H42" s="38" t="s">
+        <v>626</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>530</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>174</v>
       </c>
       <c r="K42" s="16" t="s">
-        <v>526</v>
-      </c>
-      <c r="L42" s="41">
-        <v>9</v>
+        <v>531</v>
+      </c>
+      <c r="L42" s="38">
+        <v>5</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="O42" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="P42" s="14"/>
+        <v>481</v>
+      </c>
+      <c r="P42" s="45"/>
       <c r="Q42" s="14"/>
       <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
+      <c r="S42" s="12" t="s">
+        <v>534</v>
+      </c>
       <c r="T42" s="16" t="s">
-        <v>529</v>
-      </c>
-      <c r="U42" s="41"/>
+        <v>535</v>
+      </c>
+      <c r="U42" s="38"/>
       <c r="V42" s="14"/>
       <c r="W42" s="14"/>
       <c r="X42" s="14"/>
@@ -20727,62 +20705,60 @@
       <c r="AA42" s="14"/>
       <c r="AB42" s="14"/>
     </row>
-    <row r="43" spans="1:28" ht="398.75" customHeight="1">
+    <row r="43" spans="1:28" ht="387" customHeight="1">
       <c r="A43" s="9">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>617</v>
+        <v>536</v>
       </c>
       <c r="C43" s="14">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="D43" s="46" t="s">
-        <v>522</v>
+        <v>537</v>
       </c>
       <c r="E43" s="47" t="s">
-        <v>530</v>
-      </c>
-      <c r="F43" s="9">
-        <v>2012</v>
+        <v>538</v>
+      </c>
+      <c r="F43" s="48">
+        <v>2018</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>531</v>
-      </c>
-      <c r="H43" s="41" t="s">
+        <v>539</v>
+      </c>
+      <c r="H43" s="38" t="s">
         <v>628</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="K43" s="16" t="s">
-        <v>533</v>
-      </c>
-      <c r="L43" s="41">
-        <v>5</v>
+        <v>541</v>
+      </c>
+      <c r="K43" s="38" t="s">
+        <v>632</v>
+      </c>
+      <c r="L43" s="38">
+        <v>13</v>
       </c>
       <c r="M43" s="16" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="N43" s="12" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
       <c r="O43" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="P43" s="48"/>
+        <v>481</v>
+      </c>
+      <c r="P43" s="14"/>
       <c r="Q43" s="14"/>
       <c r="R43" s="14"/>
-      <c r="S43" s="12" t="s">
-        <v>536</v>
-      </c>
+      <c r="S43" s="14"/>
       <c r="T43" s="16" t="s">
-        <v>537</v>
-      </c>
-      <c r="U43" s="41"/>
+        <v>544</v>
+      </c>
+      <c r="U43" s="38"/>
       <c r="V43" s="14"/>
       <c r="W43" s="14"/>
       <c r="X43" s="14"/>
@@ -20791,60 +20767,64 @@
       <c r="AA43" s="14"/>
       <c r="AB43" s="14"/>
     </row>
-    <row r="44" spans="1:28" ht="387" customHeight="1">
+    <row r="44" spans="1:28" ht="409.5" customHeight="1">
       <c r="A44" s="9">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
       <c r="C44" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" s="49" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="E44" s="50" t="s">
-        <v>540</v>
-      </c>
-      <c r="F44" s="51">
-        <v>2018</v>
+        <v>547</v>
+      </c>
+      <c r="F44" s="48">
+        <v>2019</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>541</v>
-      </c>
-      <c r="H44" s="41" t="s">
-        <v>630</v>
+        <v>548</v>
+      </c>
+      <c r="H44" s="38" t="s">
+        <v>44</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>543</v>
-      </c>
-      <c r="K44" s="41" t="s">
-        <v>637</v>
-      </c>
-      <c r="L44" s="41">
-        <v>13</v>
+        <v>174</v>
+      </c>
+      <c r="K44" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="L44" s="38">
+        <v>5</v>
       </c>
       <c r="M44" s="16" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="N44" s="12" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="O44" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="P44" s="14"/>
+        <v>481</v>
+      </c>
+      <c r="P44" s="12" t="s">
+        <v>553</v>
+      </c>
       <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
+      <c r="R44" s="12" t="s">
+        <v>554</v>
+      </c>
       <c r="S44" s="14"/>
-      <c r="T44" s="16" t="s">
-        <v>546</v>
-      </c>
-      <c r="U44" s="41"/>
+      <c r="T44" s="51" t="s">
+        <v>555</v>
+      </c>
+      <c r="U44" s="38"/>
       <c r="V44" s="14"/>
       <c r="W44" s="14"/>
       <c r="X44" s="14"/>
@@ -20855,62 +20835,60 @@
     </row>
     <row r="45" spans="1:28" ht="409.5" customHeight="1">
       <c r="A45" s="9">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>547</v>
+        <v>556</v>
       </c>
       <c r="C45" s="14">
-        <v>2</v>
-      </c>
-      <c r="D45" s="52" t="s">
-        <v>548</v>
-      </c>
-      <c r="E45" s="53" t="s">
-        <v>549</v>
-      </c>
-      <c r="F45" s="51">
+        <v>6</v>
+      </c>
+      <c r="D45" s="49" t="s">
+        <v>557</v>
+      </c>
+      <c r="E45" s="50" t="s">
+        <v>558</v>
+      </c>
+      <c r="F45" s="48">
         <v>2019</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>550</v>
-      </c>
-      <c r="H45" s="41" t="s">
+        <v>559</v>
+      </c>
+      <c r="H45" s="38" t="s">
         <v>44</v>
       </c>
       <c r="I45" s="16" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>174</v>
+        <v>561</v>
       </c>
       <c r="K45" s="16" t="s">
-        <v>552</v>
-      </c>
-      <c r="L45" s="41">
-        <v>5</v>
+        <v>562</v>
+      </c>
+      <c r="L45" s="38">
+        <v>10</v>
       </c>
       <c r="M45" s="16" t="s">
-        <v>553</v>
+        <v>563</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="O45" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="P45" s="12" t="s">
-        <v>555</v>
-      </c>
+        <v>481</v>
+      </c>
+      <c r="P45" s="14"/>
       <c r="Q45" s="14"/>
       <c r="R45" s="12" t="s">
-        <v>556</v>
+        <v>565</v>
       </c>
       <c r="S45" s="14"/>
-      <c r="T45" s="54" t="s">
-        <v>557</v>
-      </c>
-      <c r="U45" s="41"/>
+      <c r="T45" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="U45" s="38"/>
       <c r="V45" s="14"/>
       <c r="W45" s="14"/>
       <c r="X45" s="14"/>
@@ -20921,60 +20899,60 @@
     </row>
     <row r="46" spans="1:28" ht="409.5" customHeight="1">
       <c r="A46" s="9">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>558</v>
+        <v>567</v>
       </c>
       <c r="C46" s="14">
-        <v>6</v>
-      </c>
-      <c r="D46" s="52" t="s">
-        <v>559</v>
-      </c>
-      <c r="E46" s="53" t="s">
-        <v>560</v>
-      </c>
-      <c r="F46" s="51">
-        <v>2019</v>
+        <v>10</v>
+      </c>
+      <c r="D46" s="49" t="s">
+        <v>568</v>
+      </c>
+      <c r="E46" s="52" t="s">
+        <v>569</v>
+      </c>
+      <c r="F46" s="48">
+        <v>2018</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>561</v>
-      </c>
-      <c r="H46" s="41" t="s">
+        <v>570</v>
+      </c>
+      <c r="H46" s="38" t="s">
         <v>44</v>
       </c>
       <c r="I46" s="16" t="s">
-        <v>562</v>
+        <v>430</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>563</v>
+        <v>174</v>
       </c>
       <c r="K46" s="16" t="s">
-        <v>564</v>
-      </c>
-      <c r="L46" s="41">
-        <v>10</v>
+        <v>571</v>
+      </c>
+      <c r="L46" s="38">
+        <v>9</v>
       </c>
       <c r="M46" s="16" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="O46" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="P46" s="14"/>
+        <v>445</v>
+      </c>
+      <c r="P46" s="12" t="s">
+        <v>574</v>
+      </c>
       <c r="Q46" s="14"/>
-      <c r="R46" s="12" t="s">
-        <v>567</v>
-      </c>
+      <c r="R46" s="14"/>
       <c r="S46" s="14"/>
       <c r="T46" s="16" t="s">
-        <v>568</v>
-      </c>
-      <c r="U46" s="41"/>
+        <v>575</v>
+      </c>
+      <c r="U46" s="38"/>
       <c r="V46" s="14"/>
       <c r="W46" s="14"/>
       <c r="X46" s="14"/>
@@ -20983,62 +20961,56 @@
       <c r="AA46" s="14"/>
       <c r="AB46" s="14"/>
     </row>
-    <row r="47" spans="1:28" ht="409.5" customHeight="1">
+    <row r="47" spans="1:28" ht="337.25" customHeight="1">
       <c r="A47" s="9">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="C47" s="14">
-        <v>10</v>
-      </c>
-      <c r="D47" s="52" t="s">
-        <v>570</v>
-      </c>
-      <c r="E47" s="55" t="s">
-        <v>571</v>
-      </c>
-      <c r="F47" s="51">
-        <v>2018</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>572</v>
-      </c>
-      <c r="H47" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="49" t="s">
+        <v>577</v>
+      </c>
+      <c r="E47" s="53" t="s">
+        <v>578</v>
+      </c>
+      <c r="F47" s="48">
+        <v>2017</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>579</v>
+      </c>
+      <c r="H47" s="38" t="s">
         <v>44</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>432</v>
+        <v>580</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="K47" s="16" t="s">
-        <v>573</v>
-      </c>
-      <c r="L47" s="41">
-        <v>9</v>
+        <v>581</v>
+      </c>
+      <c r="L47" s="38">
+        <v>4</v>
       </c>
       <c r="M47" s="16" t="s">
-        <v>574</v>
-      </c>
-      <c r="N47" s="12" t="s">
-        <v>575</v>
-      </c>
-      <c r="O47" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="P47" s="12" t="s">
-        <v>576</v>
-      </c>
+        <v>582</v>
+      </c>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
       <c r="Q47" s="14"/>
       <c r="R47" s="14"/>
       <c r="S47" s="14"/>
       <c r="T47" s="16" t="s">
-        <v>577</v>
-      </c>
-      <c r="U47" s="41"/>
+        <v>583</v>
+      </c>
+      <c r="U47" s="38"/>
       <c r="V47" s="14"/>
       <c r="W47" s="14"/>
       <c r="X47" s="14"/>
@@ -21047,56 +21019,58 @@
       <c r="AA47" s="14"/>
       <c r="AB47" s="14"/>
     </row>
-    <row r="48" spans="1:28" ht="337.25" customHeight="1">
+    <row r="48" spans="1:28" ht="409.5" customHeight="1">
       <c r="A48" s="9">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>578</v>
+        <v>619</v>
       </c>
       <c r="C48" s="14">
-        <v>0</v>
-      </c>
-      <c r="D48" s="52" t="s">
-        <v>579</v>
-      </c>
-      <c r="E48" s="56" t="s">
-        <v>580</v>
-      </c>
-      <c r="F48" s="51">
-        <v>2017</v>
-      </c>
-      <c r="G48" s="35" t="s">
-        <v>581</v>
-      </c>
-      <c r="H48" s="41" t="s">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="D48" s="49" t="s">
+        <v>584</v>
+      </c>
+      <c r="E48" s="53" t="s">
+        <v>585</v>
+      </c>
+      <c r="F48" s="48">
+        <v>2019</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>586</v>
+      </c>
+      <c r="H48" s="38" t="s">
+        <v>24</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>217</v>
+        <v>588</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>583</v>
-      </c>
-      <c r="L48" s="41">
-        <v>4</v>
+        <v>589</v>
+      </c>
+      <c r="L48" s="38">
+        <v>18</v>
       </c>
       <c r="M48" s="16" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
+      <c r="O48" s="12" t="s">
+        <v>481</v>
+      </c>
       <c r="P48" s="14"/>
       <c r="Q48" s="14"/>
       <c r="R48" s="14"/>
       <c r="S48" s="14"/>
       <c r="T48" s="16" t="s">
-        <v>585</v>
-      </c>
-      <c r="U48" s="41"/>
+        <v>591</v>
+      </c>
+      <c r="U48" s="38"/>
       <c r="V48" s="14"/>
       <c r="W48" s="14"/>
       <c r="X48" s="14"/>
@@ -21104,66 +21078,6 @@
       <c r="Z48" s="14"/>
       <c r="AA48" s="14"/>
       <c r="AB48" s="14"/>
-    </row>
-    <row r="49" spans="1:28" ht="409.5" customHeight="1">
-      <c r="A49" s="9">
-        <v>40</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="C49" s="14">
-        <v>3</v>
-      </c>
-      <c r="D49" s="52" t="s">
-        <v>586</v>
-      </c>
-      <c r="E49" s="56" t="s">
-        <v>587</v>
-      </c>
-      <c r="F49" s="51">
-        <v>2019</v>
-      </c>
-      <c r="G49" s="35" t="s">
-        <v>588</v>
-      </c>
-      <c r="H49" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="I49" s="16" t="s">
-        <v>589</v>
-      </c>
-      <c r="J49" s="12" t="s">
-        <v>590</v>
-      </c>
-      <c r="K49" s="16" t="s">
-        <v>591</v>
-      </c>
-      <c r="L49" s="41">
-        <v>18</v>
-      </c>
-      <c r="M49" s="16" t="s">
-        <v>592</v>
-      </c>
-      <c r="N49" s="14"/>
-      <c r="O49" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="16" t="s">
-        <v>593</v>
-      </c>
-      <c r="U49" s="41"/>
-      <c r="V49" s="14"/>
-      <c r="W49" s="14"/>
-      <c r="X49" s="14"/>
-      <c r="Y49" s="14"/>
-      <c r="Z49" s="14"/>
-      <c r="AA49" s="14"/>
-      <c r="AB49" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -21173,15 +21087,15 @@
     <hyperlink ref="N11" r:id="rId4" display="https://github.com/arsadeghi/ACME-Generator"/>
     <hyperlink ref="V11" r:id="rId5" display="AndroidandArchitecture.InAndroidDevelopersBlog.https://android-developers"/>
     <hyperlink ref="V12" r:id="rId6" display="http://blog.hello2morrow.com/2016/08/how-to-organize-your-code"/>
-    <hyperlink ref="U24" r:id="rId7" display="http://www.sonarsource.org/evaluate-your-"/>
-    <hyperlink ref="N26" r:id="rId8" display="sourceforge.net"/>
-    <hyperlink ref="U31" r:id="rId9" display="https://doi.org/10.5381/jot.2013.12.2.a1"/>
-    <hyperlink ref="D33" r:id="rId10" display="Clemente Izurieta "/>
-    <hyperlink ref="U33" r:id="rId11" display="dagstuhl.de/16162"/>
-    <hyperlink ref="D34" r:id="rId12" display="Terese Besker "/>
-    <hyperlink ref="D35" r:id="rId13" display="Areti Ampatzoglou "/>
-    <hyperlink ref="D36" r:id="rId14" display="Antonio Martini "/>
-    <hyperlink ref="M42" r:id="rId15" display="cwe.mitre.org"/>
+    <hyperlink ref="U23" r:id="rId7" display="http://www.sonarsource.org/evaluate-your-"/>
+    <hyperlink ref="N25" r:id="rId8" display="sourceforge.net"/>
+    <hyperlink ref="U30" r:id="rId9" display="https://doi.org/10.5381/jot.2013.12.2.a1"/>
+    <hyperlink ref="D32" r:id="rId10" display="Clemente Izurieta "/>
+    <hyperlink ref="U32" r:id="rId11" display="dagstuhl.de/16162"/>
+    <hyperlink ref="D33" r:id="rId12" display="Terese Besker "/>
+    <hyperlink ref="D34" r:id="rId13" display="Areti Ampatzoglou "/>
+    <hyperlink ref="D35" r:id="rId14" display="Antonio Martini "/>
+    <hyperlink ref="M41" r:id="rId15" display="cwe.mitre.org"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <headerFooter>

</xml_diff>

<commit_message>
Updating papers and created some graphics.
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form.xlsx
+++ b/dataset/Extraction_form.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="240" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Folha 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="668">
   <si>
     <t>Citation</t>
   </si>
@@ -8053,541 +8053,6 @@
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>As subjects for this study, we used 20 Java OSS projects, which have been selected based on the following criteria</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>—</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">for more details see Arvanitou et al. [6]: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t xml:space="preserve">	- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">The software is a popular OSS project </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">in </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>sourceforge.net</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">. This criterion ensures that the investigated projects are rec- ognized as important by the OSS community. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t xml:space="preserve">	- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">The software has more than 20 versions </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">(official releases). We have included this criterion for similar reasons to c1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t xml:space="preserve">	- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>The software contains more than 300 classes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">. This criteri- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t> -on ensures that we will not include “toy examples” in our  -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">dataset. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>The software is written in java</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">. We include this criterion </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t> -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">because the employed metric calculation tools analyse Java bytecode. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t> - -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">Coupling and cohesion at the package level have been quantified using three metrics: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">ACa </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">– </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">Average Coupling Afferent </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">This metric represents the average afferent coupling of packages. Afferent cou- pling is the number of outgoing dependencies of a package to other packages [14]. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve"> -
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">TCIP </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">– </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>Total Coupling Intensity between Packages</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">: This metric represents the count of class dependencies that span among different packages. This metric is inspired by the traditional Coupling between Objects metrics [8], which is calculated at the class level. The idea of employing two coupling metrics is that one (ACa) captures the number of dependencies at the architecture level, whereas the other (TCIP) the intensity of the dependency [4]. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve"> -
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>CaPC - Cohesion among Package Classes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>: This metric assesses how closely two classes that belong to the same package collaborate with each other. The metric is inspired by reversing the calculation of Lack of Cohesion of Meth- ods [8]. To calculate this metrics we compute the total number of pairs of classes that belong to one package, and then we investigate the percentage of these pairs that are coherent (i.e., they are coupled to each other).  - -</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>Data Collection and Analysis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">. Each package of our dataset (i.e., row) is characterized by five variables: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>TD Princi- pal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>ACa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, TCIP, and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>CaPC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">. To answer the aforementioned research questions we perform: (a) Spearman and Pearson Cor- relation between </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>ACa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, TCIP and TD, and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">CaPC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">and TD Prin- cipal, (b) Univariate Regression Analysis with dependent vari- ables: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>ACa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, TCIP and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>CaPC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, and (c) hypothesis testing to check the discriminative power of TD to identify classes with low cohesion and high coupling. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">The main tool to perform the analysis was the SonarQube.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t xml:space="preserve">To achieve this goal we have performed a large-scale empirical study on more than 1,000 packages written in Java and ex- plored the aforementioned relationship. </t>
     </r>
     <r>
@@ -8891,138 +8356,6 @@
   <si>
     <r>
       <rPr>
-        <i/>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">Architectural Technical Debt (ATD) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">Visualization of ATD and Its Interest </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">Electrical Architecture at Volvo Car Group </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">It was defined three levels:  -- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">Logical View </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve"> -- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">Design View </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve"> -- </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">Deployment and Efficiency </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t> -In general, it was defined as a set of car components domain where there is a set of ECU for each specific domain, and for each ECU, there is a set of LC (Logical Component). The author defined a weight scale (0,1,2). 0 is the weight between LCs in the same ECU, 1 is the weight between LCs in deferent ECUs but in the same domain, and weight 2 means that the communication between LCs is between different ECUs deferents Domain.  - -After defined the Architecture of the components, the Architect check the deployment and compare with the original Architecture. The cost of interest is calculate according the formula proposed by the authors.  - -It was created a specific Graphic Dependency Tool to show the “Misplaced LC interest”</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="13"/>
         <color indexed="8"/>
         <rFont val="Times Roman"/>
@@ -9429,21 +8762,6 @@
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t>Design Structural Matrix -- Direct DSM  -- Visubility DSM - -Modularity -- Measure component coupling -- Measure Fan-In/Fan-out - -Maintenance costs - -Measure defect-related activity according the bug occurrence and file related to bug. - -Financial Analysis using code of line as a parameter. According the number of LOC modify. The authors proposed a spent effort of LOC changed in file.</t>
   </si>
   <si>
     <t>Empirical Study of two different systems created in C/C++ with two different architecturee. The first in a Hierarchical Architecture and the Second as a Core-Perifphery Architeture.</t>
@@ -15973,12 +15291,6 @@
     <t>Jeremy Ludwig; Steven Xu; Frederick Webber</t>
   </si>
   <si>
-    <t>Confernce</t>
-  </si>
-  <si>
-    <t>Conferene</t>
-  </si>
-  <si>
     <t>Symposium</t>
   </si>
   <si>
@@ -16004,13 +15316,823 @@
   </si>
   <si>
     <t>Computer architecture,Software engineering,Business,History,Sonar detection,Microprocessors</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>Architectural Technical Debt (ATD)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">Visualization of ATD and Its Interest </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">Electrical Architecture at Volvo Car Group </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">It was defined three levels:  +- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">Logical View </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve"> +- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">Design View </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve"> +- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">Deployment and Efficiency </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t> +In general, it was defined as a set of car components domain where there is a set of ECU for each specific domain, and for each ECU, there is a set of LC (Logical Component). The author defined a weight scale (0,1,2). 0 is the weight between LCs in the same ECU, 1 is the weight between LCs in deferent ECUs but in the same domain, and weight 2 means that the communication between LCs is between different ECUs deferents Domain.  + +After defined the Architecture of the components, the Architect check the deployment and compare with the original Architecture. The cost of interest is calculate according the formula proposed by the authors.  + +It was created a specific Graphic Dependency Tool to show the “Misplaced LC interest”</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>As subjects for this study, we used 20 Java OSS projects, which have been selected based on the following criteria</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>—</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>for more details see Arvanitou et al. [6]: Pearson, Correlations (Correlation), Spearman Correlation (Consistency) and Linear Regression (Predict Power), tool: sonarqube</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t xml:space="preserve">	- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">The software is a popular OSS project </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">in </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>sourceforge.net</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">. This criterion ensures that the investigated projects are rec- ognized as important by the OSS community. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t xml:space="preserve">	- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">The software has more than 20 versions </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">(official releases). We have included this criterion for similar reasons to c1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t xml:space="preserve">	- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>The software contains more than 300 classes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">. This criteri- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t> +on ensures that we will not include “toy examples” in our  +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">dataset. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>The software is written in java</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">. We include this criterion </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t> +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">because the employed metric calculation tools analyse Java bytecode. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t> + +</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Coupling and cohesion at the package level have been quantified using three metrics: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">ACa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">– </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">Average Coupling Afferent </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">This metric represents the average afferent coupling of packages. Afferent cou- pling is the number of outgoing dependencies of a package to other packages [14]. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve"> +
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">TCIP </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">– </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>Total Coupling Intensity between Packages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">: This metric represents the count of class dependencies that span among different packages. This metric is inspired by the traditional Coupling between Objects metrics [8], which is calculated at the class level. The idea of employing two coupling metrics is that one (ACa) captures the number of dependencies at the architecture level, whereas the other (TCIP) the intensity of the dependency [4]. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve"> +
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>CaPC - Cohesion among Package Classes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>: This metric assesses how closely two classes that belong to the same package collaborate with each other. The metric is inspired by reversing the calculation of Lack of Cohesion of Meth- ods [8]. To calculate this metrics we compute the total number of pairs of classes that belong to one package, and then we investigate the percentage of these pairs that are coherent (i.e., they are coupled to each other).  + +</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>Data Collection and Analysis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">. Each package of our dataset (i.e., row) is characterized by five variables: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>TD Princi- pal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>ACa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, TCIP, and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>CaPC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">. To answer the aforementioned research questions we perform: (a) Spearman and Pearson Cor- relation between </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>ACa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, TCIP and TD, and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">CaPC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">and TD Prin- cipal, (b) Univariate Regression Analysis with dependent vari- ables: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>ACa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, TCIP and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>CaPC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, and (c) hypothesis testing to check the discriminative power of TD to identify classes with low cohesion and high coupling. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+The main tool to perform the analysis was the SonarQube.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Package modularity via Sonaqube using TD index from cohesion and coupling.</t>
+  </si>
+  <si>
+    <t>[4] E. M. Arvanitou, A. Ampatzoglou, K. Tzouvalidis, A. Chatzigeorgiou,
+P. Avgeriou, and I. Deligiannis, “Assessing Change Proneness at the Architecture Level: An Empirical Validation”, International Workshop on Emerging Trends in Software Design and Architecture (WETSoDA 2017), IEEE, 2017.
+[5] E. M. Arvanitou, A. Ampatzoglou, A. Chatzigeorgiou, and P. Avgeriou,
+“Introducing a ripple effect measure: a theoretical and empirical validation”, 9th Int. Symposium on Empirical Software Engineering and Measurement (ESEM ‘15), IEEE, 22–23 October 2015, China.
+[6] E. M. Arvanitou, A. Ampatzoglou, A. Chatzigeorgiou, and P. Avgeriou.
+“Software Metrics Fluctuation: A Property for Assisting the Metric
+Selection Process”, Information and Software Technology, 72 (4), 2016.
+[7] E. M. Arvanitou, A. Ampatzoglou, A. Chatzigeorgiou, and P. Avgeriou, “A Method for Assessing Class Change Proneness”, 21st International Conference on Evaluation and Assessment in Software Engineering
+(EASE’ 17), ACM, 15-16 June 2017, Sweden.</t>
+  </si>
+  <si>
+    <t>The study selected popular open projects that is available; the proposed metrics are simple to calculate; the proposed correlation is easy to understand</t>
+  </si>
+  <si>
+    <t>The study shoud be provide a repliaction kit</t>
+  </si>
+  <si>
+    <t>roblem characterization: yes, bibliographic review: yes, data collection: yes, hypothesis: yes, experimentation: yes, results: yes, final: good</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>Skiada et al. 2018</t>
+  </si>
+  <si>
+    <t>There is no ADTM process, there is no how to calculate ATD cust</t>
+  </si>
+  <si>
+    <t>[3] D.Durisic,M.Nilsson,M.Staron,andJ.Hansson.Measuringtheimpact of changes to the complexity and coupling properties of automotive software systems. 86(5):1275–1293. [7] Z. Li, P. Avgeriou, and P. Liang. A systematic mapping study on technical debt and its management. Journal of Systems and Software, 101(0):193 – 220, 2015.
+[8] A. Martini, J. Bosch, and M. Chaudron. Architecture technical debt: Understanding causes and a qualitative model. In Software Engineering and Advanced Applications (SEAA), 2014 40th EUROMICRO Confer- ence on, pages 85–92, Aug 2014.
+[9] R. Nord, I. Ozkaya, P. Kruchten, and M. Gonzalez-Rojas. In search of a metric for managing architectural technical debt. In 2012 Joint Working IEEE/IFIP Conference on Software Architecture (WICSA) and European Conference on Software Architecture (ECSA), pages 91–100.</t>
+  </si>
+  <si>
+    <t>The study was performed in a real case industry application</t>
+  </si>
+  <si>
+    <t>There is no repliaction kit to reproduce the study</t>
+  </si>
+  <si>
+    <t>In this paper, we present a novel approach for visualizing the debt and the interest together. Such visualization helps the stakeholders identifying and prioritizing ATD, by under- standing the impact of different ATD items (specifically non- allowed dependencies) on efficiency. The validation interviews with the stakeholders at VCG confirmed that such tool would be valuable for architects and other stakeholders. It is important for calculate the performance communication between the components in a automotive domain, but can be used in a network distributed system such as a microservice system.</t>
+  </si>
+  <si>
+    <t>In the future we plan to continue our research on what other ATD items can be found and what other impact measures can be combined together for having the complete picture of ATD and its interest, which would greatly help the decision making of the main stakeholders. We also plan to investigate the reasoning behind the architectural violations, whatever they are intentional or not, and whatever or which the architectural violations benefit the final product. Finally, stakeholders that were part of the early evaluation of the tool said that it would be valuable to see the evolution of the debt. They wanted to see if the tendency is that the debt increases or decreases over time, as well as see what impact planned or potential future changes would have.</t>
+  </si>
+  <si>
+    <t>Since there is only one studied system, the resulting method- ology is entirely based on such studied case and could there- fore potentially be limited to similarly designed architectures, e.g. where an intended architecture is realized as logical components deployed to ECUs.</t>
+  </si>
+  <si>
+    <t>[9] Garcia, J., Popescu, D., Edwards, G., Medvidovic, N.: Identifying
+architectural bad smells. In: Proc. CSMR 2009. IEEE, Germany (2009); [12] Letouzey, J.L.: The SQALE method for evaluating technical debt. In:
+Proc. 3rd Int. Work. on Managing Technical Debt (June 2012)</t>
+  </si>
+  <si>
+    <t>In future work, we are interested in verifying how much architectural issues affect the overall quality, with the aim of giving different relevance to architecture and design issues w.r.t. coding ones in a TDI. We plan to investigate the role of code and architectural smells in TD, since they are associated to known solutions, that can speed up their resolution process. We would like also to work on the definition of a new TDI, with a focus on code and architectural debt, and experiment it on a large dataset of projects. In the TDI computation we would like to consider: 1) Code and Architectural smells detection; 2) Code and architecture/design metrics; 3) History of a system, including code changes and lifespan of smells; 4) Identification of problems more critical than others, to weight the collected analysis elements (e.g., metrics, smells, issues) according to their relevance in existing (past) projects.</t>
+  </si>
+  <si>
+    <t>roblem characterization: yes, bibliographic review: yes, data collection: yes, hypothesis: no, experimentation: no, results: yes, final: regular</t>
+  </si>
+  <si>
+    <t>It was collected five tools to check TD index about ATD. It was observed how to calculate de TD index and the unit measure.</t>
+  </si>
+  <si>
+    <t>The study should be created an experimentation using real systems to compare each tool evaluated.</t>
+  </si>
+  <si>
+    <t>There is no data collected to compare the used tools. There is no Design research and there is no an experiment to evaluate the tools using a set of data.</t>
+  </si>
+  <si>
+    <t>The cost was calculated using resolution cost. Only tools Cast and SonarGraph has a ATD index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[12] Letouzey, J.L.: The SQALE method for evaluating technical debt. In:
+Proc. 3rd Int. Work. on Managing Technical Debt (June 2012); [9] Garcia, J., Popescu, D., Edwards, G., Medvidovic, N.: Identifying
+architectural bad smells. In: Proc. CSMR 2009. IEEE, Germany (2009); </t>
+  </si>
+  <si>
+    <t>The dataset was not available to reproduce the study.</t>
+  </si>
+  <si>
+    <t>The authors studied a real case for three years and collect data from two large systems about effort and spend the maintenance. The authors analyzed the SVC repository, the bug tracker related to commits, the files changes, and refactoring propagation cust to maintain the systems.</t>
+  </si>
+  <si>
+    <t>problem characterization: yes, bibliographic review: yes, data collection: yes, hypothesis: no, experimentation: yes, results: yes, final: good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The study did not explain the architectural debt used to refactoring in architectural system maintenance. We examine only two systems, albeit with very different designs and from two different firms. We cannot be sure that the findings would apply to other firms or sys- tems. </t>
+  </si>
+  <si>
+    <t>Our study generates a number of avenues for future work. First, it provides a benchmark for future studies that seek to examine the relationship between measures of architecture and the costs associated with maintenance and adaptation. Second, it provides methods for evaluating the technical debt associated with software architecture, which could be verified via future empirical studies across a larger number of contexts and systems. Finally, while we focus only on the costs associated with corrective maintenance, a significant amount of the value from refactoring is likely to come from an increase in developer productivity when responding to new requirements. It is our hope that the methods we describe can provide a springboard for undertaking such enquiries.</t>
+  </si>
+  <si>
+    <t>Complexity, coupling and cyclical dependencies  using DSM (Dependent Structure Matrix). The time spends on maintenance.</t>
+  </si>
+  <si>
+    <t>Brooks, FrederickP., 1975. The Mythical Man-Month.; Kruchten, P, Nord, R.L., Ozkaya, M., 2012a. Technical Debt: from metaphor to theory to practice. IEEE Softw 29 (6), 18–21.
+Kruchten, P., Gonzalez, M., Ozkaya, I., Nord, R.L., Kruchten, N., 2012b. Change prop- agation as a measure of structural technical debt. WICSA/ECSA.
+Li, Z., Avgeriou, P., Liang, P., 2015. A systematic mapping on technical debt and its management. J. Syst. Softw 101, 193–220. ; Guo, Y., Seaman, C.A, 2011. Portfolio approach to technical debt management. 2nd Workshop on Managing Technical Debt. ACM.; Baldwin, C., MacCormack, A., Rusnak, J., 2014. Hidden structure: using network methods to map system architecture. Res. Policy 43 (8), 1381–1397.; MacCormack, A., Baldwin, C., Rusnak, J., 2012. Exploring the duality between prod- uct and organizational architectures: a test of the ’mirroring’ hypothesis. Res. Policy 41 (8), 1309–1324.;  MacCormack, A., Rusnak, J., Baldwin, C., 2006. Exploring the structure of complex software designs: an empirical study of open source and proprietary code. Man- age. Sci. 52 (7), 1015–1030. ; Sosa, Manuel, Eppinger, Steven, Rowles, Craig, 2007. A network approach to define modularity of components in complex products. Trans.ASME 129, 1118–1129.</t>
+  </si>
+  <si>
+    <t>The cust was based on the time spends on maintanance record in issue tracker. The authors defined a standard cost of U$ 100 per hour to calculate the cust of activity.</t>
+  </si>
+  <si>
+    <t>Design Structural Matrix +- Direct DSM  +- Visubility DSM + + Modularity +- Measure component coupling +- Measure Fan-In/Fan- costs +  +Measure defect-related activity according the bug occurrence and file related to bug. + + Financial Analysis using code of line as a parameter. According the number of LOC modify. The authors proposed a spent effort of LOC changed in file. OLR to do Regression. Refactoring.</t>
+  </si>
+  <si>
+    <t>[6] F. A. Fontana, I. Pigazzini, R. Roveda, and M. Zanoni, “Automatic detection of instability architectural smells,” Proceedings - 2016 IEEE International Conference on Software Maintenance and Evolution, IC- SME 2016, pp. 433–437, 2017.; [9] R. Roveda, F. A. Fontana, I. Pigazzini, and M. Zanoni, “Towards an architectural debt index,” in 2018 44th Euromicro Conference on Software Engineering and Advanced Applications (SEAA), pp. 408–416, IEEE, 2018.</t>
+  </si>
+  <si>
+    <t>The authors studied an evolution process of identifying and tracking architectural smells in corpus qualitas.</t>
+  </si>
+  <si>
+    <t>Architecture Smells: +- Unstable Dependency +- Hub-like Dependency +- Cyclic Dependency + +Criticality +- Reference Packages +- Dependencies +- Cycle Sharing + +PageRank + +It was used the Arcan Tool to detect the three Architecture Smells. + +Criticitality of Architec. The authors studied 14 open source java projects (from Qualitas Corpus). Data mining, evolution smells through the versions, correlation among architectural smells. ASTracker to track architectural smells evoluation. Use Jaccard Similarity index to compare set of files between analysed consecutive versions.</t>
+  </si>
+  <si>
+    <t>As future work, we plan to extend our tooling to mine archi- tectural smells directly from Git repositories, thus allowing us to link the current information to code churn and investigate the effects of smells on change rates.</t>
+  </si>
+  <si>
+    <t>The study evaluates only a few projects in java language from Qualitas Corpus. Maybe it does not apply to the industry or other software languages.</t>
+  </si>
+  <si>
+    <t>The architectural debt index using architectural smells and tracking the index's evolution throughout a system’s history was not precise; for example, the authors should be created a formula to represent the architectural debt index. They were even using a demonstration of evaluation of each architectural smell individually, but a general formula was not created.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="55" x14ac:knownFonts="1">
+  <fonts count="56" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -16311,6 +16433,12 @@
       <color indexed="23"/>
       <name val="Times Roman"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -16455,8 +16583,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
@@ -16623,7 +16763,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -17774,8 +17918,8 @@
   <dimension ref="A1:AB48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -17807,7 +17951,7 @@
   <sheetData>
     <row r="1" spans="1:28" ht="28" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -17816,52 +17960,52 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>600</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>603</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>4</v>
@@ -17870,25 +18014,25 @@
         <v>5</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>604</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="355" customHeight="1">
@@ -17902,7 +18046,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
@@ -18206,7 +18350,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="C6" s="11">
         <v>4</v>
@@ -18436,7 +18580,7 @@
         <v>129</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>623</v>
+        <v>44</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>130</v>
@@ -18648,7 +18792,7 @@
         <v>172</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>624</v>
+        <v>44</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>173</v>
@@ -18682,7 +18826,7 @@
       </c>
       <c r="S12" s="14"/>
       <c r="T12" s="14" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="U12" s="14"/>
       <c r="V12" s="12" t="s">
@@ -18790,7 +18934,7 @@
         <v>200</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>201</v>
@@ -18816,24 +18960,24 @@
       <c r="P14" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="Q14" s="14"/>
+      <c r="Q14" s="14" t="s">
+        <v>479</v>
+      </c>
       <c r="R14" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="S14" s="14"/>
+      <c r="S14" s="14" t="s">
+        <v>651</v>
+      </c>
       <c r="T14" s="10" t="s">
         <v>208</v>
       </c>
       <c r="U14" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="14"/>
+      <c r="V14" s="14" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="15" spans="1:28" ht="409.5" customHeight="1">
       <c r="A15" s="9">
@@ -19083,7 +19227,7 @@
         <v>215</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="L18" s="14">
         <v>16</v>
@@ -19146,7 +19290,7 @@
         <v>271</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>272</v>
@@ -19155,7 +19299,7 @@
         <v>273</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="L19" s="14">
         <v>4</v>
@@ -19227,7 +19371,7 @@
         <v>288</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="L20" s="14">
         <v>10</v>
@@ -19341,7 +19485,7 @@
         <v>309</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>310</v>
@@ -19540,7 +19684,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>60</v>
+        <v>637</v>
       </c>
       <c r="C25" s="9">
         <v>5</v>
@@ -19576,102 +19720,136 @@
         <v>350</v>
       </c>
       <c r="N25" s="12" t="s">
+        <v>630</v>
+      </c>
+      <c r="O25" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="O25" s="12" t="s">
+      <c r="P25" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q25" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="R25" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="12" t="s">
+      <c r="S25" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="T25" s="16" t="s">
         <v>353</v>
       </c>
-      <c r="S25" s="14"/>
-      <c r="T25" s="16" t="s">
+      <c r="U25" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="U25" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="V25" s="14"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="14"/>
-      <c r="Z25" s="14"/>
-      <c r="AA25" s="14"/>
-      <c r="AB25" s="14"/>
+      <c r="V25" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="W25" s="14" t="s">
+        <v>633</v>
+      </c>
+      <c r="X25" s="14" t="s">
+        <v>634</v>
+      </c>
+      <c r="Y25" s="14" t="s">
+        <v>635</v>
+      </c>
+      <c r="Z25" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="AA25" s="14" t="s">
+        <v>638</v>
+      </c>
+      <c r="AB25" s="14" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="26" spans="1:28" ht="409.5" customHeight="1">
       <c r="A26" s="9">
         <v>31</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C26" s="9">
         <v>17</v>
       </c>
       <c r="D26" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="E26" s="24" t="s">
         <v>357</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>358</v>
       </c>
       <c r="F26" s="9">
         <v>2015</v>
       </c>
       <c r="G26" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>621</v>
+      </c>
+      <c r="I26" s="26" t="s">
         <v>359</v>
-      </c>
-      <c r="H26" s="25" t="s">
-        <v>626</v>
-      </c>
-      <c r="I26" s="26" t="s">
-        <v>360</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>174</v>
       </c>
       <c r="K26" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L26" s="13">
         <v>8</v>
       </c>
       <c r="M26" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="O26" s="12" t="s">
         <v>362</v>
       </c>
-      <c r="N26" s="12" t="s">
+      <c r="P26" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="O26" s="12" t="s">
+      <c r="Q26" s="12" t="s">
         <v>364</v>
       </c>
-      <c r="P26" s="12" t="s">
+      <c r="R26" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="Q26" s="12" t="s">
+      <c r="S26" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="T26" s="16" t="s">
         <v>366</v>
       </c>
-      <c r="R26" s="12" t="s">
+      <c r="U26" s="12" t="s">
         <v>367</v>
       </c>
-      <c r="S26" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="T26" s="16" t="s">
-        <v>368</v>
-      </c>
-      <c r="U26" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="14"/>
-      <c r="Y26" s="14"/>
-      <c r="Z26" s="14"/>
-      <c r="AA26" s="14"/>
-      <c r="AB26" s="14"/>
+      <c r="V26" s="14" t="s">
+        <v>639</v>
+      </c>
+      <c r="W26" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="X26" s="14" t="s">
+        <v>641</v>
+      </c>
+      <c r="Y26" s="14" t="s">
+        <v>635</v>
+      </c>
+      <c r="Z26" s="14" t="s">
+        <v>642</v>
+      </c>
+      <c r="AA26" s="14" t="s">
+        <v>644</v>
+      </c>
+      <c r="AB26" s="14" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="27" spans="1:28" ht="409.5" customHeight="1">
       <c r="A27" s="9">
@@ -19687,245 +19865,299 @@
         <v>198</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F27" s="9">
         <v>2016</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J27" s="12" t="s">
         <v>174</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L27" s="13">
         <v>4</v>
       </c>
       <c r="M27" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="O27" s="12" t="s">
         <v>374</v>
-      </c>
-      <c r="N27" s="12" t="s">
-        <v>375</v>
-      </c>
-      <c r="O27" s="12" t="s">
-        <v>376</v>
       </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
       <c r="R27" s="14"/>
       <c r="S27" s="14"/>
       <c r="T27" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="14"/>
-      <c r="AB27" s="14"/>
+      <c r="V27" s="14" t="s">
+        <v>652</v>
+      </c>
+      <c r="W27" s="14" t="s">
+        <v>648</v>
+      </c>
+      <c r="X27" s="14" t="s">
+        <v>650</v>
+      </c>
+      <c r="Y27" s="14" t="s">
+        <v>647</v>
+      </c>
+      <c r="Z27" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="AA27" s="14" t="s">
+        <v>649</v>
+      </c>
+      <c r="AB27" s="14" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="28" spans="1:28" ht="358.25" customHeight="1">
       <c r="A28" s="9">
         <v>43</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C28" s="14">
         <v>35</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F28" s="29">
         <v>2016</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>24</v>
       </c>
       <c r="I28" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="K28" s="27" t="s">
         <v>380</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>381</v>
-      </c>
-      <c r="K28" s="27" t="s">
-        <v>382</v>
       </c>
       <c r="L28" s="13">
         <v>13</v>
       </c>
       <c r="M28" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>661</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="P28" s="14" t="s">
+        <v>658</v>
+      </c>
+      <c r="Q28" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="R28" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="S28" s="14" t="s">
+        <v>660</v>
+      </c>
+      <c r="T28" s="16" t="s">
         <v>383</v>
       </c>
-      <c r="N28" s="12" t="s">
+      <c r="U28" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="O28" s="12" t="s">
-        <v>385</v>
-      </c>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="U28" s="12" t="s">
-        <v>387</v>
-      </c>
-      <c r="V28" s="14"/>
-      <c r="W28" s="14"/>
-      <c r="X28" s="14"/>
-      <c r="Y28" s="14"/>
-      <c r="Z28" s="14"/>
-      <c r="AA28" s="14"/>
-      <c r="AB28" s="14"/>
+      <c r="V28" s="14" t="s">
+        <v>659</v>
+      </c>
+      <c r="W28" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="X28" s="14" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y28" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="Z28" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="AA28" s="14" t="s">
+        <v>656</v>
+      </c>
+      <c r="AB28" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="29" spans="1:28" ht="333.25" customHeight="1">
       <c r="A29" s="9">
         <v>51</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C29" s="9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F29" s="9">
         <v>2019</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>44</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="L29" s="13">
         <v>11</v>
       </c>
       <c r="M29" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="N29" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="P29" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q29" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="N29" s="14"/>
-      <c r="O29" s="12" t="s">
+      <c r="R29" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="P29" s="12" t="s">
+      <c r="S29" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="T29" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="Q29" s="12" t="s">
+      <c r="U29" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="R29" s="12" t="s">
-        <v>399</v>
-      </c>
-      <c r="S29" s="14"/>
-      <c r="T29" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="U29" s="12" t="s">
-        <v>401</v>
-      </c>
-      <c r="V29" s="14"/>
-      <c r="W29" s="14"/>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="14"/>
-      <c r="Z29" s="14"/>
-      <c r="AA29" s="14"/>
-      <c r="AB29" s="14"/>
+      <c r="V29" s="14" t="s">
+        <v>662</v>
+      </c>
+      <c r="W29" s="14" t="s">
+        <v>663</v>
+      </c>
+      <c r="X29" s="14" t="s">
+        <v>667</v>
+      </c>
+      <c r="Y29" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="Z29" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="AA29" s="14" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB29" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="30" spans="1:28" ht="409.5" customHeight="1">
       <c r="A30" s="9">
         <v>52</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C30" s="9">
         <v>3</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F30" s="9">
         <v>2019</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H30" s="13" t="s">
         <v>44</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>215</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="L30" s="13">
         <v>8</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="N30" s="12" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="P30" s="12" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="Q30" s="14"/>
       <c r="R30" s="12" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="S30" s="14"/>
       <c r="T30" s="10" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="U30" s="12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="V30" s="14"/>
       <c r="W30" s="14"/>
@@ -19940,58 +20172,58 @@
         <v>63</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C31" s="9">
         <v>4</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F31" s="9">
         <v>2019</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H31" s="33" t="s">
         <v>24</v>
       </c>
       <c r="I31" s="34" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="J31" s="12" t="s">
         <v>131</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="L31" s="13">
         <v>31</v>
       </c>
       <c r="M31" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="O31" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="P31" s="12" t="s">
         <v>420</v>
-      </c>
-      <c r="N31" s="12" t="s">
-        <v>421</v>
-      </c>
-      <c r="O31" s="12" t="s">
-        <v>422</v>
-      </c>
-      <c r="P31" s="12" t="s">
-        <v>423</v>
       </c>
       <c r="Q31" s="14"/>
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
       <c r="T31" s="10" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="U31" s="12" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="V31" s="14"/>
       <c r="W31" s="14"/>
@@ -20006,60 +20238,60 @@
         <v>73</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C32" s="9">
         <v>8</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F32" s="9">
         <v>2018</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="H32" s="33" t="s">
         <v>44</v>
       </c>
       <c r="I32" s="34" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="J32" s="12" t="s">
         <v>174</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="L32" s="13">
         <v>5</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="O32" s="14"/>
       <c r="P32" s="12" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="Q32" s="14"/>
       <c r="R32" s="12" t="s">
         <v>250</v>
       </c>
       <c r="S32" s="12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="T32" s="10" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="U32" s="12" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="V32" s="14"/>
       <c r="W32" s="14"/>
@@ -20074,62 +20306,62 @@
         <v>69</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C33" s="9">
         <v>21</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E33" s="35" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F33" s="9">
         <v>2017</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="H33" s="33" t="s">
         <v>44</v>
       </c>
       <c r="I33" s="34" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="L33" s="13">
         <v>11</v>
       </c>
       <c r="M33" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="P33" s="12" t="s">
         <v>443</v>
-      </c>
-      <c r="N33" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="O33" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="P33" s="12" t="s">
-        <v>446</v>
       </c>
       <c r="Q33" s="14"/>
       <c r="R33" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="S33" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="T33" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="U33" s="12" t="s">
         <v>447</v>
-      </c>
-      <c r="S33" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="T33" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="U33" s="12" t="s">
-        <v>450</v>
       </c>
       <c r="V33" s="14"/>
       <c r="W33" s="14"/>
@@ -20144,56 +20376,56 @@
         <v>67</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C34" s="9">
         <v>28</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F34" s="9">
         <v>2016</v>
       </c>
       <c r="G34" s="36" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H34" s="33" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="I34" s="34" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>174</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="L34" s="13">
         <v>8</v>
       </c>
       <c r="M34" s="10" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="O34" s="12" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="P34" s="14"/>
       <c r="Q34" s="14"/>
       <c r="R34" s="14"/>
       <c r="S34" s="14"/>
       <c r="T34" s="16" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="U34" s="16" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="V34" s="14"/>
       <c r="W34" s="14"/>
@@ -20208,56 +20440,56 @@
         <v>66</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C35" s="9">
         <v>12</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E35" s="37" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F35" s="9">
         <v>2016</v>
       </c>
       <c r="G35" s="36" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="H35" s="33" t="s">
         <v>44</v>
       </c>
       <c r="I35" s="34" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>288</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="L35" s="13">
         <v>8</v>
       </c>
       <c r="M35" s="10" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="O35" s="12" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="P35" s="14"/>
       <c r="Q35" s="14"/>
       <c r="R35" s="14"/>
       <c r="S35" s="14"/>
       <c r="T35" s="16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="U35" s="16" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="V35" s="14"/>
       <c r="W35" s="14"/>
@@ -20272,61 +20504,61 @@
         <v>96</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C36" s="9">
         <v>0</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E36" s="37" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F36" s="9">
         <v>2017</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H36" s="33" t="s">
         <v>44</v>
       </c>
       <c r="I36" s="34" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="L36" s="38">
         <v>10</v>
       </c>
       <c r="M36" s="16" t="s">
+        <v>476</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="P36" s="12" t="s">
         <v>479</v>
       </c>
-      <c r="N36" s="12" t="s">
+      <c r="Q36" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="O36" s="12" t="s">
+      <c r="R36" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="S36" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="T36" s="16" t="s">
         <v>481</v>
-      </c>
-      <c r="P36" s="12" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q36" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="R36" s="12" t="s">
-        <v>482</v>
-      </c>
-      <c r="S36" s="12" t="s">
-        <v>482</v>
-      </c>
-      <c r="T36" s="16" t="s">
-        <v>484</v>
       </c>
       <c r="U36" s="38"/>
       <c r="V36" s="14"/>
@@ -20342,53 +20574,53 @@
         <v>35</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C37" s="9">
         <v>65</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="F37" s="9">
         <v>2015</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="H37" s="33" t="s">
         <v>24</v>
       </c>
       <c r="I37" s="34" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="K37" s="39" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="L37" s="38">
         <v>17</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="O37" s="12" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="P37" s="14"/>
       <c r="Q37" s="14"/>
       <c r="R37" s="14"/>
       <c r="S37" s="14"/>
       <c r="T37" s="16" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="U37" s="38"/>
       <c r="V37" s="14"/>
@@ -20404,43 +20636,43 @@
         <v>24</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C38" s="9">
         <v>15</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E38" s="40" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F38" s="9">
         <v>2018</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="H38" s="54" t="s">
         <v>44</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>131</v>
       </c>
       <c r="K38" s="39" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="L38" s="38">
         <v>27</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="O38" s="14"/>
       <c r="P38" s="14"/>
@@ -20448,7 +20680,7 @@
       <c r="R38" s="14"/>
       <c r="S38" s="14"/>
       <c r="T38" s="16" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="U38" s="38"/>
       <c r="V38" s="14"/>
@@ -20464,43 +20696,43 @@
         <v>77</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C39" s="9">
         <v>9</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F39" s="9">
         <v>2019</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="H39" s="25" t="s">
         <v>44</v>
       </c>
       <c r="I39" s="26" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="K39" s="39" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="L39" s="38">
         <v>11</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="O39" s="14"/>
       <c r="P39" s="14"/>
@@ -20508,7 +20740,7 @@
       <c r="R39" s="14"/>
       <c r="S39" s="14"/>
       <c r="T39" s="16" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="U39" s="38"/>
       <c r="V39" s="14"/>
@@ -20524,43 +20756,43 @@
         <v>78</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C40" s="14">
         <v>12</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F40" s="9">
         <v>2017</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="H40" s="25" t="s">
         <v>44</v>
       </c>
       <c r="I40" s="26" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="J40" s="14" t="s">
         <v>131</v>
       </c>
       <c r="K40" s="16" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="L40" s="38">
         <v>5</v>
       </c>
       <c r="M40" s="16" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="O40" s="14"/>
       <c r="P40" s="14"/>
@@ -20568,7 +20800,7 @@
       <c r="R40" s="14"/>
       <c r="S40" s="14"/>
       <c r="T40" s="16" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="U40" s="38"/>
       <c r="V40" s="14"/>
@@ -20584,53 +20816,53 @@
         <v>81</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C41" s="14">
         <v>105</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F41" s="9">
         <v>2012</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H41" s="25" t="s">
         <v>24</v>
       </c>
       <c r="I41" s="26" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>174</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="L41" s="38">
         <v>9</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="O41" s="12" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="P41" s="14"/>
       <c r="Q41" s="14"/>
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
       <c r="T41" s="16" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="U41" s="38"/>
       <c r="V41" s="14"/>
@@ -20646,55 +20878,55 @@
         <v>82</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C42" s="14">
         <v>103</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E42" s="44" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F42" s="9">
         <v>2012</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H42" s="38" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>174</v>
       </c>
       <c r="K42" s="16" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="L42" s="38">
         <v>5</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="N42" s="12" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="O42" s="12" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="P42" s="45"/>
       <c r="Q42" s="14"/>
       <c r="R42" s="14"/>
       <c r="S42" s="12" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="T42" s="16" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="U42" s="38"/>
       <c r="V42" s="14"/>
@@ -20710,53 +20942,53 @@
         <v>85</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C43" s="14">
         <v>1</v>
       </c>
       <c r="D43" s="46" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E43" s="47" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F43" s="48">
         <v>2018</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="H43" s="38" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="K43" s="38" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="L43" s="38">
         <v>13</v>
       </c>
       <c r="M43" s="16" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="N43" s="12" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="O43" s="12" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="P43" s="14"/>
       <c r="Q43" s="14"/>
       <c r="R43" s="14"/>
       <c r="S43" s="14"/>
       <c r="T43" s="16" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="U43" s="38"/>
       <c r="V43" s="14"/>
@@ -20772,57 +21004,57 @@
         <v>88</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C44" s="14">
         <v>2</v>
       </c>
       <c r="D44" s="49" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E44" s="50" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F44" s="48">
         <v>2019</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="H44" s="38" t="s">
         <v>44</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>174</v>
       </c>
       <c r="K44" s="16" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="L44" s="38">
         <v>5</v>
       </c>
       <c r="M44" s="16" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="N44" s="12" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="O44" s="12" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="P44" s="12" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="Q44" s="14"/>
       <c r="R44" s="12" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="S44" s="14"/>
       <c r="T44" s="51" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="U44" s="38"/>
       <c r="V44" s="14"/>
@@ -20838,55 +21070,55 @@
         <v>90</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C45" s="14">
         <v>6</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E45" s="50" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="F45" s="48">
         <v>2019</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="H45" s="38" t="s">
         <v>44</v>
       </c>
       <c r="I45" s="16" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="K45" s="16" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="L45" s="38">
         <v>10</v>
       </c>
       <c r="M45" s="16" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="O45" s="12" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="P45" s="14"/>
       <c r="Q45" s="14"/>
       <c r="R45" s="12" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="S45" s="14"/>
       <c r="T45" s="16" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="U45" s="38"/>
       <c r="V45" s="14"/>
@@ -20902,55 +21134,55 @@
         <v>91</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C46" s="14">
         <v>10</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E46" s="52" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="F46" s="48">
         <v>2018</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="H46" s="38" t="s">
         <v>44</v>
       </c>
       <c r="I46" s="16" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>174</v>
       </c>
       <c r="K46" s="16" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="L46" s="38">
         <v>9</v>
       </c>
       <c r="M46" s="16" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="O46" s="12" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="P46" s="12" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="Q46" s="14"/>
       <c r="R46" s="14"/>
       <c r="S46" s="14"/>
       <c r="T46" s="16" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="U46" s="38"/>
       <c r="V46" s="14"/>
@@ -20966,40 +21198,40 @@
         <v>97</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="C47" s="14">
         <v>0</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E47" s="53" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="F47" s="48">
         <v>2017</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="H47" s="38" t="s">
         <v>44</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="J47" s="12" t="s">
         <v>215</v>
       </c>
       <c r="K47" s="16" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="L47" s="38">
         <v>4</v>
       </c>
       <c r="M47" s="16" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="N47" s="14"/>
       <c r="O47" s="14"/>
@@ -21008,7 +21240,7 @@
       <c r="R47" s="14"/>
       <c r="S47" s="14"/>
       <c r="T47" s="16" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="U47" s="38"/>
       <c r="V47" s="14"/>
@@ -21024,51 +21256,51 @@
         <v>40</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C48" s="14">
         <v>3</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E48" s="53" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F48" s="48">
         <v>2019</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H48" s="38" t="s">
         <v>24</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="L48" s="38">
         <v>18</v>
       </c>
       <c r="M48" s="16" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="N48" s="14"/>
       <c r="O48" s="12" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="P48" s="14"/>
       <c r="Q48" s="14"/>
       <c r="R48" s="14"/>
       <c r="S48" s="14"/>
       <c r="T48" s="16" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="U48" s="38"/>
       <c r="V48" s="14"/>

</xml_diff>

<commit_message>
Update dataset and utilities
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form.xlsx
+++ b/dataset/Extraction_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="0" windowWidth="25140" windowHeight="15020"/>
+    <workbookView xWindow="140" yWindow="0" windowWidth="33460" windowHeight="20020"/>
   </bookViews>
   <sheets>
     <sheet name="Folha 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="719">
   <si>
     <t>Citation</t>
   </si>
@@ -10884,9 +10884,6 @@
     <t>Survey and interviews with practionners from Skandinavia software industry area.</t>
   </si>
   <si>
-    <t>36% of effort in Software development cycle is effort about TD.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="13"/>
@@ -11232,158 +11229,6 @@
         <rFont val="Times New Roman"/>
       </rPr>
       <t xml:space="preserve">IEEE 8th International Workshop on Managing Technical Debt </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">To check how practitioners percept Technical Debt in Embedded Systems about Quality Attributes. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>RQ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">What is the relationship between the expected lifetime of components and technical debt? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>RQ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">What types of technical debt (e.g., code, architectural, etc.) are more frequently occurring in embedded sys- tems? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>RQ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">What is the significance of building maintainable soft- ware systems (with low TD) compared to satisfying other quality attributes?  - -Case study in seven technology companies:  -Telecomunication -Automotive -Mobile -Sensors -Priting -Smart Manufacturing -Media Devices </t>
     </r>
     <r>
       <rPr>
@@ -16096,6 +15941,198 @@
   <si>
     <t xml:space="preserve">International Workshop on Managing Technical Debt (MTD)
 </t>
+  </si>
+  <si>
+    <t>[33] E. Tom, A. Aurum, and R. Vidgen, “An exploration of technical debt,” Journal of Systems and Software, vol. 86, no. 6, 2013, pp. 1498-1516.; [1] A. Ampatzoglou, A. Ampatzoglou, A. Chatzigeorgiou, and P. Avgeriou, “The financial aspect of managing technical debt: A systematic literature review,” Information and Software Technology, vol. 64, 2015, pp. 52.</t>
+  </si>
+  <si>
+    <t>36% of effort in Software development cycle is effort about whole TD.</t>
+  </si>
+  <si>
+    <t>This is the first study surveying the estimated magnitude of the interest paid on the accumulated TD in terms of perceived wasted time and effort. The study has shown that software development practitioners estimate that 36 % of all development time is wasted due to TD and that Complex Architectural Design and Requirement TD generates the most negative impact on daily software development work.</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>The qualitative data derived from the survey are not based on measured or observed data but on estimations made by the respondents. In future studies, we plan to include physical measurements and observations, to create a stronger reliability of the data. The result of this research may be affected by some threats to validity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The qualitative data derived from the survey are not based on measured or observed data but on estimations made by the respondents. </t>
+  </si>
+  <si>
+    <t>Good, due to demonstrate how important is the effort waste with TD (36%) and the study showed that Software Architecture and Requirements are the aspects most important because waste more time to fix TD.</t>
+  </si>
+  <si>
+    <t>problem characterization: yes, bibliographic review: yes, data collection: yes, hypothesis: no, experimentation: no, results: yes, final: good</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To check how practitioners percept Technical Debt in Embedded Systems about Quality Attributes. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>RQ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">What is the relationship between the expected lifetime of components and technical debt? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>RQ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">What types of technical debt (e.g., code, architectural, etc.) are more frequently occurring in embedded sys- tems? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>RQ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">What is the significance of building maintainable software systems (with low TD) compared to satisfying other quality attributes?  + +Case study in seven technology companies:  +Telecomunication + Automotive + Mobile + Sensors + Priting + Smart Manufacturing + Media Devices </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Yes, it was evaluated each version about a lot of types of TD, including ATD. However, the ATD was identified manually via interviews.</t>
+  </si>
+  <si>
+    <t>It was used interviews for each company</t>
+  </si>
+  <si>
+    <t>problem characterization: yes, bibliographic review: yes, data collection: yes, hypothesis: yes, experimentation: no, results: yes, final: good</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Good, due to Architectural Technical Debt's findings as an essential kind of TD that happens in the context of embedded systems.</t>
+  </si>
+  <si>
+    <t>The study did not show how to measure the TD.</t>
+  </si>
+  <si>
+    <t>The study collected real data from a real industry of software embedded using questionaries and interviews about the effort spent on Technical Debt in the embedded system. Thus, the study identified that test TD, code TD, and Architectural TD were highlighted as main kinds of TD, and qualities attributes as functionality, reliability, and performance were the most important in this context.</t>
+  </si>
+  <si>
+    <t>There are no details about how to identify the TD, and there are no explicit future works.</t>
   </si>
 </sst>
 </file>
@@ -16548,8 +16585,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -16734,12 +16774,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -17890,8 +17931,8 @@
   <dimension ref="A1:AC48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -17923,7 +17964,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="28" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -17932,55 +17973,55 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>573</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>574</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>576</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>579</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>581</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>4</v>
@@ -17989,25 +18030,25 @@
         <v>5</v>
       </c>
       <c r="W1" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>591</v>
-      </c>
       <c r="Z1" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>583</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="355" customHeight="1">
@@ -18021,7 +18062,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>7</v>
@@ -18115,7 +18156,7 @@
         <v>24</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>25</v>
@@ -18280,7 +18321,7 @@
         <v>63</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="M5" s="11">
         <v>4</v>
@@ -18337,7 +18378,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C6" s="11">
         <v>4</v>
@@ -18361,7 +18402,7 @@
         <v>82</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>44</v>
@@ -18436,7 +18477,7 @@
         <v>97</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>98</v>
@@ -18511,13 +18552,13 @@
         <v>113</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>114</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="M8" s="14">
         <v>10</v>
@@ -18582,7 +18623,7 @@
         <v>126</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>127</v>
@@ -18657,7 +18698,7 @@
         <v>142</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>127</v>
@@ -18732,7 +18773,7 @@
         <v>156</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>157</v>
@@ -18809,7 +18850,7 @@
         <v>170</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="M12" s="13">
         <v>2</v>
@@ -18834,7 +18875,7 @@
       </c>
       <c r="T12" s="14"/>
       <c r="U12" s="14" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="V12" s="14"/>
       <c r="W12" s="12" t="s">
@@ -18945,19 +18986,19 @@
         <v>195</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>196</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>197</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="M14" s="13">
         <v>3</v>
@@ -18975,13 +19016,13 @@
         <v>201</v>
       </c>
       <c r="R14" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="S14" s="12" t="s">
         <v>134</v>
       </c>
       <c r="T14" s="14" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="U14" s="10" t="s">
         <v>202</v>
@@ -18990,7 +19031,7 @@
         <v>203</v>
       </c>
       <c r="W14" s="14" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="409.5" customHeight="1">
@@ -19022,7 +19063,7 @@
         <v>208</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>209</v>
@@ -19100,7 +19141,7 @@
         <v>236</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="L16" s="10" t="s">
         <v>224</v>
@@ -19247,13 +19288,13 @@
         <v>251</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>209</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="M18" s="14">
         <v>16</v>
@@ -19316,19 +19357,19 @@
         <v>264</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>265</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="M19" s="14">
         <v>4</v>
@@ -19397,13 +19438,13 @@
         <v>279</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>280</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="M20" s="14">
         <v>10</v>
@@ -19520,7 +19561,7 @@
         <v>301</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>302</v>
@@ -19541,7 +19582,7 @@
         <v>305</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>209</v>
@@ -19608,7 +19649,7 @@
         <v>316</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="K23" s="12" t="s">
         <v>209</v>
@@ -19677,13 +19718,13 @@
         <v>327</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>170</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="M24" s="14">
         <v>2</v>
@@ -19728,7 +19769,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C25" s="9">
         <v>5</v>
@@ -19752,13 +19793,13 @@
         <v>339</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="K25" s="12" t="s">
         <v>127</v>
       </c>
       <c r="L25" s="27" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="M25" s="13">
         <v>4</v>
@@ -19767,22 +19808,22 @@
         <v>340</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="P25" s="12" t="s">
         <v>341</v>
       </c>
       <c r="Q25" s="14" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="R25" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="S25" s="12" t="s">
         <v>342</v>
       </c>
       <c r="T25" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="U25" s="16" t="s">
         <v>343</v>
@@ -19791,25 +19832,25 @@
         <v>344</v>
       </c>
       <c r="W25" s="14" t="s">
+        <v>609</v>
+      </c>
+      <c r="X25" s="14" t="s">
+        <v>610</v>
+      </c>
+      <c r="Y25" s="14" t="s">
         <v>611</v>
       </c>
-      <c r="X25" s="14" t="s">
+      <c r="Z25" s="14" t="s">
         <v>612</v>
       </c>
-      <c r="Y25" s="14" t="s">
+      <c r="AA25" s="14" t="s">
         <v>613</v>
       </c>
-      <c r="Z25" s="14" t="s">
-        <v>614</v>
-      </c>
-      <c r="AA25" s="14" t="s">
+      <c r="AB25" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="AB25" s="14" t="s">
-        <v>617</v>
-      </c>
       <c r="AC25" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="26" spans="1:29" ht="409.5" customHeight="1">
@@ -19835,13 +19876,13 @@
         <v>348</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I26" s="26" t="s">
         <v>349</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>170</v>
@@ -19856,7 +19897,7 @@
         <v>351</v>
       </c>
       <c r="O26" s="12" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="P26" s="12" t="s">
         <v>352</v>
@@ -19880,25 +19921,25 @@
         <v>357</v>
       </c>
       <c r="W26" s="14" t="s">
+        <v>616</v>
+      </c>
+      <c r="X26" s="14" t="s">
+        <v>617</v>
+      </c>
+      <c r="Y26" s="14" t="s">
         <v>618</v>
       </c>
-      <c r="X26" s="14" t="s">
+      <c r="Z26" s="14" t="s">
+        <v>612</v>
+      </c>
+      <c r="AA26" s="14" t="s">
         <v>619</v>
       </c>
-      <c r="Y26" s="14" t="s">
+      <c r="AB26" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="AC26" s="14" t="s">
         <v>620</v>
-      </c>
-      <c r="Z26" s="14" t="s">
-        <v>614</v>
-      </c>
-      <c r="AA26" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="AB26" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="AC26" s="14" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="409.5" customHeight="1">
@@ -19924,13 +19965,13 @@
         <v>359</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>360</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="K27" s="12" t="s">
         <v>170</v>
@@ -19959,25 +20000,25 @@
       </c>
       <c r="V27" s="14"/>
       <c r="W27" s="14" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="X27" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="Y27" s="14" t="s">
         <v>627</v>
       </c>
-      <c r="Y27" s="14" t="s">
-        <v>629</v>
-      </c>
       <c r="Z27" s="14" t="s">
+        <v>624</v>
+      </c>
+      <c r="AA27" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="AB27" s="14" t="s">
         <v>626</v>
       </c>
-      <c r="AA27" s="14" t="s">
-        <v>615</v>
-      </c>
-      <c r="AB27" s="14" t="s">
-        <v>628</v>
-      </c>
       <c r="AC27" s="14" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="358.25" customHeight="1">
@@ -19985,13 +20026,13 @@
         <v>43</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C28" s="14">
         <v>35</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>366</v>
@@ -20009,7 +20050,7 @@
         <v>368</v>
       </c>
       <c r="J28" s="26" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>369</v>
@@ -20024,22 +20065,22 @@
         <v>371</v>
       </c>
       <c r="O28" s="12" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="P28" s="12" t="s">
         <v>372</v>
       </c>
       <c r="Q28" s="14" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="R28" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="S28" s="14" t="s">
         <v>342</v>
       </c>
       <c r="T28" s="14" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="U28" s="16" t="s">
         <v>373</v>
@@ -20048,25 +20089,25 @@
         <v>374</v>
       </c>
       <c r="W28" s="14" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="X28" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="Y28" s="14" t="s">
+        <v>630</v>
+      </c>
+      <c r="Z28" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA28" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="AB28" s="14" t="s">
         <v>633</v>
       </c>
-      <c r="Y28" s="14" t="s">
-        <v>632</v>
-      </c>
-      <c r="Z28" s="14" t="s">
+      <c r="AC28" s="14" t="s">
         <v>634</v>
-      </c>
-      <c r="AA28" s="14" t="s">
-        <v>615</v>
-      </c>
-      <c r="AB28" s="14" t="s">
-        <v>635</v>
-      </c>
-      <c r="AC28" s="14" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="333.25" customHeight="1">
@@ -20098,7 +20139,7 @@
         <v>379</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="K29" s="12" t="s">
         <v>380</v>
@@ -20113,7 +20154,7 @@
         <v>382</v>
       </c>
       <c r="O29" s="14" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="P29" s="12" t="s">
         <v>383</v>
@@ -20128,7 +20169,7 @@
         <v>386</v>
       </c>
       <c r="T29" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="U29" s="10" t="s">
         <v>387</v>
@@ -20137,25 +20178,25 @@
         <v>388</v>
       </c>
       <c r="W29" s="14" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="X29" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="Y29" s="14" t="s">
+        <v>644</v>
+      </c>
+      <c r="Z29" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="AA29" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="AB29" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="AC29" s="14" t="s">
         <v>642</v>
-      </c>
-      <c r="Y29" s="14" t="s">
-        <v>646</v>
-      </c>
-      <c r="Z29" s="14" t="s">
-        <v>634</v>
-      </c>
-      <c r="AA29" s="14" t="s">
-        <v>615</v>
-      </c>
-      <c r="AB29" s="14" t="s">
-        <v>645</v>
-      </c>
-      <c r="AC29" s="14" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="409.5" customHeight="1">
@@ -20187,7 +20228,7 @@
         <v>393</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>209</v>
@@ -20309,7 +20350,7 @@
         <v>8</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E32" s="31" t="s">
         <v>414</v>
@@ -20327,7 +20368,7 @@
         <v>416</v>
       </c>
       <c r="J32" s="34" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>170</v>
@@ -20345,13 +20386,13 @@
         <v>419</v>
       </c>
       <c r="P32" s="14" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="Q32" s="12" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="R32" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="S32" s="12" t="s">
         <v>243</v>
@@ -20366,25 +20407,25 @@
         <v>422</v>
       </c>
       <c r="W32" s="14" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="X32" s="14" t="s">
+        <v>648</v>
+      </c>
+      <c r="Y32" s="14" t="s">
+        <v>649</v>
+      </c>
+      <c r="Z32" s="14" t="s">
         <v>650</v>
       </c>
-      <c r="Y32" s="14" t="s">
+      <c r="AA32" s="14" t="s">
         <v>651</v>
       </c>
-      <c r="Z32" s="14" t="s">
+      <c r="AB32" s="14" t="s">
         <v>652</v>
       </c>
-      <c r="AA32" s="14" t="s">
-        <v>653</v>
-      </c>
-      <c r="AB32" s="14" t="s">
-        <v>654</v>
-      </c>
       <c r="AC32" s="14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="409.5" customHeight="1">
@@ -20392,13 +20433,13 @@
         <v>69</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C33" s="9">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="E33" s="35" t="s">
         <v>423</v>
@@ -20439,154 +20480,190 @@
       <c r="Q33" s="12" t="s">
         <v>430</v>
       </c>
-      <c r="R33" s="14"/>
+      <c r="R33" s="14" t="s">
+        <v>461</v>
+      </c>
       <c r="S33" s="12" t="s">
         <v>431</v>
       </c>
       <c r="T33" s="12" t="s">
+        <v>704</v>
+      </c>
+      <c r="U33" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="U33" s="10" t="s">
+      <c r="V33" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="V33" s="12" t="s">
-        <v>434</v>
-      </c>
       <c r="W33" s="14"/>
-      <c r="X33" s="14"/>
-      <c r="Y33" s="14"/>
-      <c r="Z33" s="14"/>
-      <c r="AA33" s="14"/>
-      <c r="AB33" s="14"/>
-      <c r="AC33" s="14"/>
+      <c r="X33" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="Y33" s="14" t="s">
+        <v>706</v>
+      </c>
+      <c r="Z33" s="14" t="s">
+        <v>710</v>
+      </c>
+      <c r="AA33" s="14" t="s">
+        <v>709</v>
+      </c>
+      <c r="AB33" s="14" t="s">
+        <v>708</v>
+      </c>
+      <c r="AC33" s="14" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="34" spans="1:29" ht="409.5" customHeight="1">
       <c r="A34" s="9">
         <v>67</v>
       </c>
       <c r="B34" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="C34" s="9">
+        <v>33</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>656</v>
+      </c>
+      <c r="E34" s="31" t="s">
         <v>435</v>
-      </c>
-      <c r="C34" s="9">
-        <v>28</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>658</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>436</v>
       </c>
       <c r="F34" s="9">
         <v>2016</v>
       </c>
       <c r="G34" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="H34" s="33" t="s">
+        <v>598</v>
+      </c>
+      <c r="I34" s="34" t="s">
         <v>437</v>
       </c>
-      <c r="H34" s="33" t="s">
-        <v>600</v>
-      </c>
-      <c r="I34" s="34" t="s">
-        <v>438</v>
-      </c>
       <c r="J34" s="34" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>170</v>
       </c>
       <c r="L34" s="16" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="M34" s="13">
         <v>8</v>
       </c>
       <c r="N34" s="10" t="s">
+        <v>711</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="P34" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="O34" s="12" t="s">
+      <c r="Q34" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="R34" s="14" t="s">
+        <v>712</v>
+      </c>
+      <c r="S34" s="14" t="s">
+        <v>713</v>
+      </c>
+      <c r="T34" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="U34" s="16" t="s">
         <v>440</v>
       </c>
-      <c r="P34" s="12" t="s">
+      <c r="V34" s="16" t="s">
         <v>441</v>
       </c>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-      <c r="T34" s="14"/>
-      <c r="U34" s="16" t="s">
-        <v>442</v>
-      </c>
-      <c r="V34" s="16" t="s">
-        <v>443</v>
-      </c>
       <c r="W34" s="14"/>
-      <c r="X34" s="14"/>
-      <c r="Y34" s="14"/>
-      <c r="Z34" s="14"/>
-      <c r="AA34" s="14"/>
-      <c r="AB34" s="14"/>
-      <c r="AC34" s="14"/>
+      <c r="X34" s="14" t="s">
+        <v>717</v>
+      </c>
+      <c r="Y34" s="14" t="s">
+        <v>718</v>
+      </c>
+      <c r="Z34" s="14" t="s">
+        <v>714</v>
+      </c>
+      <c r="AA34" s="14" t="s">
+        <v>715</v>
+      </c>
+      <c r="AB34" s="14" t="s">
+        <v>716</v>
+      </c>
+      <c r="AC34" s="14" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="35" spans="1:29" ht="409.5" customHeight="1">
       <c r="A35" s="9">
         <v>66</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C35" s="9">
         <v>12</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E35" s="37" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F35" s="9">
         <v>2016</v>
       </c>
       <c r="G35" s="36" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H35" s="33" t="s">
         <v>42</v>
       </c>
       <c r="I35" s="34" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J35" s="34" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K35" s="12" t="s">
         <v>280</v>
       </c>
       <c r="L35" s="16" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="M35" s="13">
         <v>8</v>
       </c>
       <c r="N35" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="P35" s="12" t="s">
         <v>449</v>
-      </c>
-      <c r="O35" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="P35" s="12" t="s">
-        <v>451</v>
       </c>
       <c r="Q35" s="14"/>
       <c r="R35" s="14"/>
       <c r="S35" s="14"/>
       <c r="T35" s="14"/>
       <c r="U35" s="16" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="V35" s="16" t="s">
-        <v>453</v>
-      </c>
-      <c r="W35" s="14"/>
+        <v>451</v>
+      </c>
+      <c r="W35" s="14" t="s">
+        <v>703</v>
+      </c>
       <c r="X35" s="14"/>
       <c r="Y35" s="14"/>
       <c r="Z35" s="14"/>
@@ -20599,64 +20676,64 @@
         <v>96</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C36" s="9">
         <v>0</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E36" s="37" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F36" s="9">
         <v>2017</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H36" s="33" t="s">
         <v>42</v>
       </c>
       <c r="I36" s="34" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="J36" s="34" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M36" s="38">
         <v>10</v>
       </c>
       <c r="N36" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="P36" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="O36" s="12" t="s">
+      <c r="Q36" s="12" t="s">
         <v>461</v>
       </c>
-      <c r="P36" s="12" t="s">
+      <c r="R36" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="Q36" s="12" t="s">
+      <c r="S36" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="T36" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="U36" s="16" t="s">
         <v>463</v>
-      </c>
-      <c r="R36" s="12" t="s">
-        <v>464</v>
-      </c>
-      <c r="S36" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="T36" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="U36" s="16" t="s">
-        <v>465</v>
       </c>
       <c r="V36" s="38"/>
       <c r="W36" s="14"/>
@@ -20672,56 +20749,56 @@
         <v>35</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C37" s="9">
         <v>65</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F37" s="9">
         <v>2015</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H37" s="33" t="s">
         <v>23</v>
       </c>
       <c r="I37" s="34" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J37" s="34" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="L37" s="39" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="M37" s="38">
         <v>17</v>
       </c>
       <c r="N37" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="O37" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="P37" s="12" t="s">
         <v>471</v>
-      </c>
-      <c r="O37" s="12" t="s">
-        <v>472</v>
-      </c>
-      <c r="P37" s="12" t="s">
-        <v>473</v>
       </c>
       <c r="Q37" s="14"/>
       <c r="R37" s="14"/>
       <c r="S37" s="14"/>
       <c r="T37" s="14"/>
       <c r="U37" s="16" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="V37" s="38"/>
       <c r="W37" s="14"/>
@@ -20737,46 +20814,46 @@
         <v>24</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C38" s="9">
         <v>15</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E38" s="40" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F38" s="9">
         <v>2018</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H38" s="54" t="s">
         <v>42</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J38" s="55" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>127</v>
       </c>
       <c r="L38" s="39" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="M38" s="38">
         <v>27</v>
       </c>
       <c r="N38" s="16" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="O38" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="P38" s="14"/>
       <c r="Q38" s="14"/>
@@ -20784,7 +20861,7 @@
       <c r="S38" s="14"/>
       <c r="T38" s="14"/>
       <c r="U38" s="16" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="V38" s="38"/>
       <c r="W38" s="14"/>
@@ -20800,46 +20877,46 @@
         <v>77</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C39" s="9">
         <v>9</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F39" s="9">
         <v>2019</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H39" s="25" t="s">
         <v>42</v>
       </c>
       <c r="I39" s="26" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="J39" s="26" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="K39" s="12" t="s">
         <v>380</v>
       </c>
       <c r="L39" s="39" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="M39" s="38">
         <v>11</v>
       </c>
       <c r="N39" s="16" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="O39" s="12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="P39" s="14"/>
       <c r="Q39" s="14"/>
@@ -20847,7 +20924,7 @@
       <c r="S39" s="14"/>
       <c r="T39" s="14"/>
       <c r="U39" s="16" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="V39" s="38"/>
       <c r="W39" s="14"/>
@@ -20863,46 +20940,46 @@
         <v>78</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C40" s="14">
         <v>12</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F40" s="9">
         <v>2017</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H40" s="25" t="s">
         <v>42</v>
       </c>
       <c r="I40" s="26" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="J40" s="26" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="K40" s="14" t="s">
         <v>127</v>
       </c>
       <c r="L40" s="16" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="M40" s="38">
         <v>5</v>
       </c>
       <c r="N40" s="16" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="O40" s="12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="P40" s="14"/>
       <c r="Q40" s="14"/>
@@ -20910,7 +20987,7 @@
       <c r="S40" s="14"/>
       <c r="T40" s="14"/>
       <c r="U40" s="16" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="V40" s="38"/>
       <c r="W40" s="14"/>
@@ -20926,56 +21003,56 @@
         <v>81</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C41" s="14">
         <v>105</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F41" s="9">
         <v>2012</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H41" s="25" t="s">
         <v>23</v>
       </c>
       <c r="I41" s="26" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="J41" s="26" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="K41" s="12" t="s">
         <v>170</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="M41" s="38">
         <v>9</v>
       </c>
       <c r="N41" s="16" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="O41" s="12" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Q41" s="14"/>
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
       <c r="T41" s="14"/>
       <c r="U41" s="16" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="V41" s="38"/>
       <c r="W41" s="14"/>
@@ -20991,58 +21068,58 @@
         <v>82</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C42" s="14">
         <v>103</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E42" s="44" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F42" s="9">
         <v>2012</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H42" s="38" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>170</v>
       </c>
       <c r="L42" s="16" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="M42" s="38">
         <v>5</v>
       </c>
       <c r="N42" s="16" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="O42" s="12" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P42" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Q42" s="45"/>
       <c r="R42" s="14"/>
       <c r="S42" s="14"/>
       <c r="T42" s="12" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="U42" s="16" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="V42" s="38"/>
       <c r="W42" s="14"/>
@@ -21058,56 +21135,56 @@
         <v>85</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C43" s="14">
         <v>1</v>
       </c>
       <c r="D43" s="46" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="E43" s="47" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F43" s="48">
         <v>2018</v>
       </c>
       <c r="G43" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="H43" s="38" t="s">
+        <v>600</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="J43" s="16" t="s">
+        <v>683</v>
+      </c>
+      <c r="K43" s="12" t="s">
         <v>518</v>
       </c>
-      <c r="H43" s="38" t="s">
-        <v>602</v>
-      </c>
-      <c r="I43" s="16" t="s">
-        <v>519</v>
-      </c>
-      <c r="J43" s="16" t="s">
-        <v>685</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>520</v>
-      </c>
       <c r="L43" s="38" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="M43" s="38">
         <v>13</v>
       </c>
       <c r="N43" s="16" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="O43" s="12" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="P43" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Q43" s="14"/>
       <c r="R43" s="14"/>
       <c r="S43" s="14"/>
       <c r="T43" s="14"/>
       <c r="U43" s="16" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="V43" s="38"/>
       <c r="W43" s="14"/>
@@ -21123,28 +21200,28 @@
         <v>88</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C44" s="14">
         <v>2</v>
       </c>
       <c r="D44" s="49" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E44" s="50" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F44" s="48">
         <v>2019</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H44" s="38" t="s">
         <v>42</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="J44" s="16" t="s">
         <v>169</v>
@@ -21153,30 +21230,30 @@
         <v>170</v>
       </c>
       <c r="L44" s="16" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="M44" s="38">
         <v>5</v>
       </c>
       <c r="N44" s="16" t="s">
+        <v>528</v>
+      </c>
+      <c r="O44" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="P44" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="Q44" s="12" t="s">
         <v>530</v>
-      </c>
-      <c r="O44" s="12" t="s">
-        <v>531</v>
-      </c>
-      <c r="P44" s="12" t="s">
-        <v>462</v>
-      </c>
-      <c r="Q44" s="12" t="s">
-        <v>532</v>
       </c>
       <c r="R44" s="14"/>
       <c r="S44" s="12" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="T44" s="14"/>
       <c r="U44" s="51" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="V44" s="38"/>
       <c r="W44" s="14"/>
@@ -21192,58 +21269,58 @@
         <v>90</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C45" s="14">
         <v>6</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E45" s="50" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F45" s="48">
         <v>2019</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H45" s="38" t="s">
         <v>42</v>
       </c>
       <c r="I45" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>684</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>537</v>
+      </c>
+      <c r="L45" s="16" t="s">
         <v>538</v>
-      </c>
-      <c r="J45" s="16" t="s">
-        <v>686</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>539</v>
-      </c>
-      <c r="L45" s="16" t="s">
-        <v>540</v>
       </c>
       <c r="M45" s="38">
         <v>10</v>
       </c>
       <c r="N45" s="16" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="O45" s="12" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="P45" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Q45" s="14"/>
       <c r="R45" s="14"/>
       <c r="S45" s="12" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="T45" s="14"/>
       <c r="U45" s="16" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="V45" s="38"/>
       <c r="W45" s="14"/>
@@ -21259,22 +21336,22 @@
         <v>91</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C46" s="14">
         <v>10</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E46" s="52" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F46" s="48">
         <v>2018</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="H46" s="38" t="s">
         <v>42</v>
@@ -21283,34 +21360,34 @@
         <v>416</v>
       </c>
       <c r="J46" s="16" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>170</v>
       </c>
       <c r="L46" s="16" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="M46" s="38">
         <v>9</v>
       </c>
       <c r="N46" s="16" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="O46" s="12" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="P46" s="12" t="s">
         <v>429</v>
       </c>
       <c r="Q46" s="12" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="R46" s="14"/>
       <c r="S46" s="14"/>
       <c r="T46" s="14"/>
       <c r="U46" s="16" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="V46" s="38"/>
       <c r="W46" s="14"/>
@@ -21326,43 +21403,43 @@
         <v>97</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C47" s="14">
         <v>0</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E47" s="53" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F47" s="48">
         <v>2017</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H47" s="38" t="s">
         <v>42</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J47" s="16" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="K47" s="12" t="s">
         <v>209</v>
       </c>
       <c r="L47" s="16" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="M47" s="38">
         <v>4</v>
       </c>
       <c r="N47" s="16" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="O47" s="14"/>
       <c r="P47" s="14"/>
@@ -21371,7 +21448,7 @@
       <c r="S47" s="14"/>
       <c r="T47" s="14"/>
       <c r="U47" s="16" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="V47" s="38"/>
       <c r="W47" s="14"/>
@@ -21387,54 +21464,54 @@
         <v>40</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C48" s="14">
         <v>3</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E48" s="53" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F48" s="48">
         <v>2019</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="H48" s="38" t="s">
         <v>23</v>
       </c>
       <c r="I48" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>686</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="L48" s="16" t="s">
         <v>565</v>
-      </c>
-      <c r="J48" s="16" t="s">
-        <v>688</v>
-      </c>
-      <c r="K48" s="12" t="s">
-        <v>566</v>
-      </c>
-      <c r="L48" s="16" t="s">
-        <v>567</v>
       </c>
       <c r="M48" s="38">
         <v>18</v>
       </c>
       <c r="N48" s="16" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="O48" s="14"/>
       <c r="P48" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="Q48" s="14"/>
       <c r="R48" s="14"/>
       <c r="S48" s="14"/>
       <c r="T48" s="14"/>
       <c r="U48" s="16" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="V48" s="38"/>
       <c r="W48" s="14"/>
@@ -21464,7 +21541,6 @@
     <hyperlink ref="N41" r:id="rId15" display="cwe.mitre.org"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>